<commit_message>
cree la rama resultadosexcelpython, ya cree una forma de exportar los resultados de arbolu a una hoa de excel, ahora lo hare en bosque y asi sucesivamente
</commit_message>
<xml_diff>
--- a/resultadospython.xlsx
+++ b/resultadospython.xlsx
@@ -1,80 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a57f4c5e645b2417/1 A NMI/3 InvestigacionMia/F Métodos predictivos con ML/A Codigo/Comparacion_de_metodos_predictivos/crispy-invention_metodos/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_496D5ECF8344E8CEE320243656245E3FB48F8CD5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D5F93C7-BF18-4916-80C4-E0C9E55C2776}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="6150" yWindow="4575" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="turnou" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
-  <si>
-    <t>Profundidad óptima arbolu</t>
-  </si>
-  <si>
-    <t>Arreglo aleatorio óptimo arbolu</t>
-  </si>
-  <si>
-    <t>Exactitud media arbolu</t>
-  </si>
-  <si>
-    <t>Desviación estándar de la exactitud arbolu</t>
-  </si>
-  <si>
-    <t>Exactitud arbolu</t>
-  </si>
-  <si>
-    <t>Precisión arbolu</t>
-  </si>
-  <si>
-    <t>Sensibilidad arbolu</t>
-  </si>
-  <si>
-    <t>F1-score arbolu</t>
-  </si>
-  <si>
-    <t>ROC/AUC arbolu</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -89,43 +47,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -413,143 +421,125 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="B2:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="2">
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>Profundidad óptima arbolu</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>Arreglo aleatorio óptimo arbolu</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>Exactitud media arbolu</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0.6086956521739131</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="1" t="inlineStr">
+        <is>
+          <t>Desviación estándar de la exactitud arbolu</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>4</v>
-      </c>
-      <c r="B2">
-        <v>38</v>
-      </c>
-      <c r="C2">
-        <v>0.60869565217391308</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0.60869565217391308</v>
-      </c>
-      <c r="F2">
-        <v>0.63833992094861669</v>
-      </c>
-      <c r="G2">
-        <v>0.60869565217391308</v>
-      </c>
-      <c r="H2">
-        <v>0.49596273291925469</v>
-      </c>
-      <c r="I2">
-        <v>0.76023944549464406</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7">
-        <v>0.60869565217391308</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9">
-        <v>0.60869565217391308</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10">
-        <v>0.63833992094861669</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11">
-        <v>0.60869565217391308</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12">
-        <v>0.49596273291925469</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13">
-        <v>0.76023944549464406</v>
+    </row>
+    <row r="6">
+      <c r="B6" s="1" t="inlineStr">
+        <is>
+          <t>Exactitud arbolu</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>0.6086956521739131</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="1" t="inlineStr">
+        <is>
+          <t>Precisión arbolu</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>0.6383399209486167</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="1" t="inlineStr">
+        <is>
+          <t>Sensibilidad arbolu</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>0.6086956521739131</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="1" t="inlineStr">
+        <is>
+          <t>F1-score arbolu</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>0.4959627329192547</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="1" t="inlineStr">
+        <is>
+          <t>ROC/AUC arbolu</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>0.7602394454946441</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
exportando resultados de metricas a excel parte 2
</commit_message>
<xml_diff>
--- a/resultadospython.xlsx
+++ b/resultadospython.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="turnou" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="knnpp" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -444,7 +444,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:C10"/>
+  <dimension ref="B2:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,91 +455,61 @@
     <row r="2">
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>Profundidad óptima arbolu</t>
+          <t>K óptimo knnpp</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t>Arreglo aleatorio óptimo arbolu</t>
+          <t>Arreglo aleatorio óptimo knnpp</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>38</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>Exactitud media arbolu</t>
+          <t>MAE knnpp</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.6086956521739131</v>
+        <v>0.7066677097061078</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>Desviación estándar de la exactitud arbolu</t>
+          <t>MSE knnpp</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>1.165834308865758</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>Exactitud arbolu</t>
+          <t>RMSE knnpp</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.6086956521739131</v>
+        <v>1.079738074194736</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>Precisión arbolu</t>
+          <t>R-cuadrado knnpp</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.6383399209486167</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" s="1" t="inlineStr">
-        <is>
-          <t>Sensibilidad arbolu</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>0.6086956521739131</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="1" t="inlineStr">
-        <is>
-          <t>F1-score arbolu</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>0.4959627329192547</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" s="1" t="inlineStr">
-        <is>
-          <t>ROC/AUC arbolu</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>0.7602394454946441</v>
+        <v>0.1742914713936639</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
borre las ramas en desuso y ahora voy a trabajar en una que se llama dev_plots para hacer las graficas y ya terminar
</commit_message>
<xml_diff>
--- a/resultadospython.xlsx
+++ b/resultadospython.xlsx
@@ -2749,22 +2749,22 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B2" t="n">
-        <v>73</v>
+        <v>141</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4116253326092697</v>
+        <v>0.6371500747583697</v>
       </c>
       <c r="D2" t="n">
-        <v>0.242363532097373</v>
+        <v>0.5827834163807639</v>
       </c>
       <c r="E2" t="n">
-        <v>0.492304308428611</v>
+        <v>0.7634025257888292</v>
       </c>
       <c r="F2" t="n">
-        <v>0.6509439320075292</v>
+        <v>0.06027717482050421</v>
       </c>
     </row>
   </sheetData>
@@ -2820,22 +2820,22 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B2" t="n">
-        <v>73</v>
+        <v>141</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4529795053261044</v>
+        <v>0.4649502752480864</v>
       </c>
       <c r="D2" t="n">
-        <v>0.3078557508588072</v>
+        <v>0.3627717795584061</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5548475023452906</v>
+        <v>0.6023053872898748</v>
       </c>
       <c r="F2" t="n">
-        <v>0.556620928182909</v>
+        <v>0.415040112673201</v>
       </c>
     </row>
   </sheetData>
@@ -2894,19 +2894,19 @@
         <v>7</v>
       </c>
       <c r="B2" t="n">
-        <v>141</v>
+        <v>38</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5631376923369429</v>
+        <v>0.7350670775892014</v>
       </c>
       <c r="D2" t="n">
-        <v>0.6470681496306073</v>
+        <v>0.7878212258727322</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8044054634514906</v>
+        <v>0.8875929392873358</v>
       </c>
       <c r="F2" t="n">
-        <v>0.06205656402289805</v>
+        <v>0.2196529674477486</v>
       </c>
     </row>
   </sheetData>
@@ -2962,22 +2962,22 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" t="n">
         <v>141</v>
       </c>
       <c r="C2" t="n">
-        <v>0.653444704720309</v>
+        <v>0.5954445053546944</v>
       </c>
       <c r="D2" t="n">
-        <v>1.068794866098178</v>
+        <v>0.8330168955623509</v>
       </c>
       <c r="E2" t="n">
-        <v>1.033825355704811</v>
+        <v>0.9126975926134302</v>
       </c>
       <c r="F2" t="n">
-        <v>0.2309800600109728</v>
+        <v>0.2402945822555412</v>
       </c>
     </row>
   </sheetData>
@@ -3033,22 +3033,22 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B2" t="n">
         <v>141</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4512870407818563</v>
+        <v>0.456863285031173</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5102636228384259</v>
+        <v>0.5143437335846587</v>
       </c>
       <c r="E2" t="n">
-        <v>0.714327391913838</v>
+        <v>0.7171776164832939</v>
       </c>
       <c r="F2" t="n">
-        <v>0.632854803984674</v>
+        <v>0.6299190801888896</v>
       </c>
     </row>
   </sheetData>
@@ -3104,22 +3104,22 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B2" t="n">
         <v>141</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7034980724585362</v>
+        <v>0.6175794785234507</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9133986034350577</v>
+        <v>0.7743973631321944</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9557188935220742</v>
+        <v>0.8799985017783806</v>
       </c>
       <c r="F2" t="n">
-        <v>0.3427908745819465</v>
+        <v>0.2937551742436224</v>
       </c>
     </row>
   </sheetData>
@@ -3252,16 +3252,16 @@
         <v>141</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5579714008453226</v>
+        <v>0.5609322990703484</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5038784557938416</v>
+        <v>0.5091111489312204</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7098439658078679</v>
+        <v>0.7135202512411406</v>
       </c>
       <c r="F2" t="n">
-        <v>0.373458798411112</v>
+        <v>0.3669522732597754</v>
       </c>
     </row>
   </sheetData>
@@ -3323,16 +3323,16 @@
         <v>73</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7066677097061078</v>
+        <v>0.7417394081863822</v>
       </c>
       <c r="D2" t="n">
-        <v>1.165834308865758</v>
+        <v>1.077288484588244</v>
       </c>
       <c r="E2" t="n">
-        <v>1.079738074194736</v>
+        <v>1.037925086212027</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1742914713936639</v>
+        <v>0.1720426223806321</v>
       </c>
     </row>
   </sheetData>
@@ -4204,25 +4204,25 @@
         <v>38</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6086956521739131</v>
+        <v>0.5686274509803922</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>0.09998077477632913</v>
       </c>
       <c r="E2" t="n">
-        <v>0.6086956521739131</v>
+        <v>0.7058823529411765</v>
       </c>
       <c r="F2" t="n">
-        <v>0.6383399209486167</v>
+        <v>0.6602434077079107</v>
       </c>
       <c r="G2" t="n">
-        <v>0.6086956521739131</v>
+        <v>0.7058823529411765</v>
       </c>
       <c r="H2" t="n">
-        <v>0.4959627329192547</v>
+        <v>0.6384803921568627</v>
       </c>
       <c r="I2" t="n">
-        <v>0.7602394454946441</v>
+        <v>0.8295847750865052</v>
       </c>
     </row>
   </sheetData>
@@ -4293,31 +4293,31 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B2" t="n">
         <v>73</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6376811594202899</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="D2" t="n">
-        <v>0.04099169746008968</v>
+        <v>0.04999038738816457</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7391304347826086</v>
+        <v>0.6764705882352942</v>
       </c>
       <c r="F2" t="n">
-        <v>0.6413043478260869</v>
+        <v>0.7005347593582888</v>
       </c>
       <c r="G2" t="n">
-        <v>0.7391304347826086</v>
+        <v>0.6764705882352942</v>
       </c>
       <c r="H2" t="n">
-        <v>0.6851574212893553</v>
+        <v>0.666547106647537</v>
       </c>
       <c r="I2" t="n">
-        <v>0.9010712035286703</v>
+        <v>0.8760092272202998</v>
       </c>
     </row>
   </sheetData>
@@ -4394,25 +4394,25 @@
         <v>38</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5652173913043478</v>
+        <v>0.5588235294117647</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5652173913043478</v>
+        <v>0.5588235294117647</v>
       </c>
       <c r="F2" t="n">
-        <v>0.3194706994328922</v>
+        <v>0.3122837370242215</v>
       </c>
       <c r="G2" t="n">
-        <v>0.5652173913043478</v>
+        <v>0.5588235294117647</v>
       </c>
       <c r="H2" t="n">
-        <v>0.4082125603864735</v>
+        <v>0.4006659267480577</v>
       </c>
       <c r="I2" t="n">
-        <v>0.8103339634530562</v>
+        <v>0.8166089965397924</v>
       </c>
     </row>
   </sheetData>
@@ -4468,22 +4468,22 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>141</v>
+        <v>73</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4933198198741591</v>
+        <v>0.5366620114553465</v>
       </c>
       <c r="D2" t="n">
-        <v>0.4994093053153734</v>
+        <v>0.4870547248066527</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7066889735345907</v>
+        <v>0.6978930611538223</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.03384695823337625</v>
+        <v>0.1796952182466954</v>
       </c>
     </row>
   </sheetData>
@@ -4545,16 +4545,16 @@
         <v>141</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3552027025235232</v>
+        <v>0.3900736969775532</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2819238313334188</v>
+        <v>0.3016540288647431</v>
       </c>
       <c r="E2" t="n">
-        <v>0.530965000102096</v>
+        <v>0.5492303968870833</v>
       </c>
       <c r="F2" t="n">
-        <v>0.4163783246019102</v>
+        <v>0.2828324552765196</v>
       </c>
     </row>
   </sheetData>
@@ -4616,16 +4616,16 @@
         <v>141</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4582086594736258</v>
+        <v>0.4210041135149655</v>
       </c>
       <c r="D2" t="n">
-        <v>0.3912001229230129</v>
+        <v>0.3372007051283547</v>
       </c>
       <c r="E2" t="n">
-        <v>0.6254599291105809</v>
+        <v>0.5806898527857661</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1901611507036736</v>
+        <v>0.1983219893132574</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
escribiendo 7aml, despues inicio con tablas
</commit_message>
<xml_diff>
--- a/resultadospython.xlsx
+++ b/resultadospython.xlsx
@@ -1,41 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27203"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a57f4c5e645b2417/1 A NMI/3 InvestigacionMia/F Métodos predictivos con ML/A Codigo/Comparacion_de_metodos_predictivos/crispy-invention_metodos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a57f4c5e645b2417/1 A NMI/3 InvestigacionMia/F Métodos predictivos con ML/A Codigo/Comparacion_de_metodos_predictivos/crispy-invention_metodos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="93" documentId="11_493A7C9B7A23541B89156E9EE9B76E285BAFCDB4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3172427-7112-8C44-9F91-A47D28999E01}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="11_2F71BF5063D29E6ADAD22262E9427B3D4E35B995" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B25081AE-4943-41DD-94BE-1D011D1847CA}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="640" windowWidth="30240" windowHeight="17780" tabRatio="895" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-90" windowWidth="29040" windowHeight="15720" tabRatio="895" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ResltCategoricas" sheetId="1" r:id="rId1"/>
     <sheet name="ResltNumericas" sheetId="2" r:id="rId2"/>
-    <sheet name="arbolu" sheetId="3" r:id="rId3"/>
-    <sheet name="bosqueu" sheetId="4" r:id="rId4"/>
-    <sheet name="knnu" sheetId="5" r:id="rId5"/>
-    <sheet name="arbolts" sheetId="6" r:id="rId6"/>
-    <sheet name="bosquets" sheetId="7" r:id="rId7"/>
-    <sheet name="knnts" sheetId="8" r:id="rId8"/>
-    <sheet name="arboltd" sheetId="9" r:id="rId9"/>
-    <sheet name="bosquetd" sheetId="10" r:id="rId10"/>
-    <sheet name="knntd" sheetId="11" r:id="rId11"/>
-    <sheet name="arbolcc" sheetId="12" r:id="rId12"/>
-    <sheet name="bosquecc" sheetId="13" r:id="rId13"/>
-    <sheet name="knncc" sheetId="14" r:id="rId14"/>
-    <sheet name="arbolpp" sheetId="15" r:id="rId15"/>
-    <sheet name="bosquepp" sheetId="16" r:id="rId16"/>
-    <sheet name="knnpp" sheetId="17" r:id="rId17"/>
+    <sheet name="Hoja1" sheetId="18" r:id="rId3"/>
+    <sheet name="arbolu" sheetId="3" r:id="rId4"/>
+    <sheet name="bosqueu" sheetId="4" r:id="rId5"/>
+    <sheet name="knnu" sheetId="5" r:id="rId6"/>
+    <sheet name="arbolts" sheetId="6" r:id="rId7"/>
+    <sheet name="bosquets" sheetId="7" r:id="rId8"/>
+    <sheet name="knnts" sheetId="8" r:id="rId9"/>
+    <sheet name="arboltd" sheetId="9" r:id="rId10"/>
+    <sheet name="bosquetd" sheetId="10" r:id="rId11"/>
+    <sheet name="knntd" sheetId="11" r:id="rId12"/>
+    <sheet name="arbolcc" sheetId="12" r:id="rId13"/>
+    <sheet name="bosquecc" sheetId="13" r:id="rId14"/>
+    <sheet name="knncc" sheetId="14" r:id="rId15"/>
+    <sheet name="arbolpp" sheetId="15" r:id="rId16"/>
+    <sheet name="bosquepp" sheetId="16" r:id="rId17"/>
+    <sheet name="knnpp" sheetId="17" r:id="rId18"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -52,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="135">
   <si>
     <t>..</t>
   </si>
@@ -463,7 +461,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -475,7 +473,6 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -515,15 +512,39 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="34">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
@@ -648,11 +669,11 @@
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Arreglo aleatorio óptimo"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Exactitud media"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Desviación estándar de la exactitud"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Exactitud" dataDxfId="25"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Precisión" dataDxfId="24"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Sensibilidad" dataDxfId="23"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="F1-score" dataDxfId="22"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="ROC/AUC" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Exactitud" dataDxfId="33"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Precisión" dataDxfId="32"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Sensibilidad" dataDxfId="31"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="F1-score" dataDxfId="30"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="ROC/AUC" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -665,10 +686,10 @@
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="tension sistolia"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Profundidad óptima"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Arreglo aleatorio óptimo"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="RMSE" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="MAE" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="R2" dataDxfId="18"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="MSE" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="RMSE" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="MAE" dataDxfId="27"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="R2" dataDxfId="26"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="MSE" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -681,10 +702,10 @@
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="tension diastolica"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Profundidad óptima"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Arreglo aleatorio óptimo"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="RMSE" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="MAE" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="R2" dataDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="MSE" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="RMSE" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="MAE" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="R2" dataDxfId="22"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="MSE" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -697,10 +718,10 @@
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="circunferencia de cintura"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Profundidad óptima"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Arreglo aleatorio óptimo"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="RMSE" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="MAE" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="R2" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="MSE" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="RMSE" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="MAE" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="R2" dataDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="MSE" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -713,31 +734,63 @@
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="perimetro de pantorrilla"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Profundidad óptima"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Arreglo aleatorio óptimo"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="RMSE" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="MAE" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="R2" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="MSE" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="RMSE" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="MAE" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="R2" dataDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="MSE" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{64211FED-7AEE-4325-B5A7-6CD161AC88BE}" name="Tabla137" displayName="Tabla137" ref="B22:K25" totalsRowShown="0">
-  <autoFilter ref="B22:K25" xr:uid="{64211FED-7AEE-4325-B5A7-6CD161AC88BE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Tabla137" displayName="Tabla137" ref="B22:K25" totalsRowShown="0">
+  <autoFilter ref="B22:K25" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{3A4D2FA9-0E5B-48D7-A3C3-A5ADB226646B}" name="turno"/>
-    <tableColumn id="2" xr3:uid="{30FD5D9F-DD9F-424C-B2C7-33A9F4BCDD07}" name="Hiperparametro"/>
-    <tableColumn id="3" xr3:uid="{6B3CE381-5309-4538-A7B8-4BFFD42B4923}" name="Arreglo aleatorio óptimo"/>
-    <tableColumn id="4" xr3:uid="{78E6B257-3B14-4375-8304-A0B022200F2D}" name="Exactitud media"/>
-    <tableColumn id="5" xr3:uid="{BE554A03-888F-4E60-9373-F4DDACC8354D}" name="Desviación estándar de la exactitud"/>
-    <tableColumn id="6" xr3:uid="{D5447D82-8811-42C6-B49A-761459B57048}" name="Exactitud" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{3C4BF4BB-D647-46EB-8F9E-E854780FAA73}" name="Precisión" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{F2F19460-4185-4B3B-A180-483E35F58B0D}" name="Sensibilidad" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{777050C1-117F-446C-ADC4-4B5E5372EB68}" name="F1-score" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{7EE9F68B-AC98-4A8C-948D-303AEF71947F}" name="ROC/AUC" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="turno"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Hiperparametro"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Arreglo aleatorio óptimo"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Exactitud media"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Desviación estándar de la exactitud"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Exactitud" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Precisión" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="Sensibilidad" dataDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0500-000009000000}" name="F1-score" dataDxfId="9"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0500-00000A000000}" name="ROC/AUC" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{399AE562-B3E6-4D52-97AF-0CCEDE975333}" name="Tabla7" displayName="Tabla7" ref="C2:I17" totalsRowShown="0">
+  <autoFilter ref="C2:I17" xr:uid="{399AE562-B3E6-4D52-97AF-0CCEDE975333}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{8A7C68C5-7F20-4474-BE9C-BB8500461A55}" name="tension sistolia"/>
+    <tableColumn id="2" xr3:uid="{56BB8918-8F80-4992-AFEC-0D3796667871}" name="Profundidad óptima"/>
+    <tableColumn id="3" xr3:uid="{73D1B751-2006-4B81-A587-07ED290E20FD}" name="Arreglo aleatorio óptimo"/>
+    <tableColumn id="4" xr3:uid="{52F0D647-D285-4F53-8571-60364FF61EB4}" name="RMSE" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{430D7FF4-20BE-4B44-B8A5-131D5AE6DA59}" name="MAE" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{2F5C611D-00DA-41C9-B3A9-A41663BE25AE}" name="R2" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{BCCAFA57-2640-4014-8DC7-6DA9812510DE}" name="MSE" dataDxfId="4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{EC235839-2E1D-45FA-9A65-CEA56421C25E}" name="Tabla79" displayName="Tabla79" ref="C20:I35" totalsRowShown="0">
+  <autoFilter ref="C20:I35" xr:uid="{EC235839-2E1D-45FA-9A65-CEA56421C25E}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{149BEF1E-16EB-4EFF-A68A-98718D3F229D}" name="tension sistolia"/>
+    <tableColumn id="2" xr3:uid="{3679D4B6-497E-455A-BE6D-18C5B33C88D5}" name="Profundidad óptima"/>
+    <tableColumn id="3" xr3:uid="{DC6B7824-ABD2-4592-9B48-EE0C932B0ED3}" name="Arreglo aleatorio óptimo"/>
+    <tableColumn id="4" xr3:uid="{D82887A3-B994-419C-AC9A-D6E7B6A6C842}" name="RMSE" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{7D98D1C3-EEA7-442A-9EE4-E922EB973C7B}" name="MAE" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{4B42BB4C-8765-4415-A7D0-B0979658564A}" name="R2" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{C54C01D6-E754-4035-A8D9-EE482DFEFC4D}" name="MSE" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1035,7 +1088,7 @@
       <selection activeCell="C3" sqref="C3:K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" customWidth="1"/>
@@ -1045,12 +1098,12 @@
     <col min="9" max="9" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -1082,7 +1135,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>11</v>
       </c>
@@ -1102,28 +1155,28 @@
         <f>arbolu!D2</f>
         <v>9.9980774776329134E-2</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="1">
         <f>arbolu!E2</f>
         <v>0.70588235294117652</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="1">
         <f>arbolu!F2</f>
         <v>0.66024340770791068</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="1">
         <f>arbolu!G2</f>
         <v>0.70588235294117652</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="1">
         <f>arbolu!H2</f>
         <v>0.6384803921568627</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="1">
         <f>arbolu!I2</f>
         <v>0.82958477508650519</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>12</v>
       </c>
@@ -1143,28 +1196,28 @@
         <f>bosqueu!D2</f>
         <v>4.9990387388164567E-2</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="1">
         <f>bosqueu!E2</f>
         <v>0.67647058823529416</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="1">
         <f>bosqueu!F2</f>
         <v>0.70053475935828879</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="1">
         <f>bosqueu!G2</f>
         <v>0.67647058823529416</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="1">
         <f>bosqueu!H2</f>
         <v>0.66654710664753702</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="1">
         <f>bosqueu!I2</f>
         <v>0.87600922722029984</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>13</v>
       </c>
@@ -1184,23 +1237,23 @@
         <f>knnu!D2</f>
         <v>0</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="1">
         <f>knnu!E2</f>
         <v>0.55882352941176472</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="1">
         <f>knnu!F2</f>
         <v>0.31228373702422152</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="1">
         <f>knnu!G2</f>
         <v>0.55882352941176472</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="1">
         <f>knnu!H2</f>
         <v>0.40066592674805768</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="1">
         <f>knnu!I2</f>
         <v>0.81660899653979235</v>
       </c>
@@ -1274,51 +1327,51 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>119</v>
+        <v>16</v>
       </c>
       <c r="B2">
         <v>141</v>
       </c>
       <c r="C2">
-        <v>0.46495027524808641</v>
+        <v>0.63715007475836971</v>
       </c>
       <c r="D2">
-        <v>0.36277177955840612</v>
+        <v>0.58278341638076392</v>
       </c>
       <c r="E2">
-        <v>0.60230538728987482</v>
+        <v>0.76340252578882917</v>
       </c>
       <c r="F2">
-        <v>0.41504011267320101</v>
+        <v>6.0277174820504209E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1327,51 +1380,51 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>7</v>
+        <v>119</v>
       </c>
       <c r="B2">
-        <v>38</v>
+        <v>141</v>
       </c>
       <c r="C2">
-        <v>0.73506707758920142</v>
+        <v>0.46495027524808641</v>
       </c>
       <c r="D2">
-        <v>0.78782122587273218</v>
+        <v>0.36277177955840612</v>
       </c>
       <c r="E2">
-        <v>0.88759293928733585</v>
+        <v>0.60230538728987482</v>
       </c>
       <c r="F2">
-        <v>0.21965296744774859</v>
+        <v>0.41504011267320101</v>
       </c>
     </row>
   </sheetData>
@@ -1380,51 +1433,51 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2">
-        <v>141</v>
+        <v>38</v>
       </c>
       <c r="C2">
-        <v>0.5954445053546944</v>
+        <v>0.73506707758920142</v>
       </c>
       <c r="D2">
-        <v>0.83301689556235092</v>
+        <v>0.78782122587273218</v>
       </c>
       <c r="E2">
-        <v>0.9126975926134302</v>
+        <v>0.88759293928733585</v>
       </c>
       <c r="F2">
-        <v>0.24029458225554121</v>
+        <v>0.21965296744774859</v>
       </c>
     </row>
   </sheetData>
@@ -1433,51 +1486,51 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>109</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>141</v>
       </c>
       <c r="C2">
-        <v>0.45686328503117302</v>
+        <v>0.5954445053546944</v>
       </c>
       <c r="D2">
-        <v>0.51434373358465868</v>
+        <v>0.83301689556235092</v>
       </c>
       <c r="E2">
-        <v>0.71717761648329392</v>
+        <v>0.9126975926134302</v>
       </c>
       <c r="F2">
-        <v>0.62991908018888965</v>
+        <v>0.24029458225554121</v>
       </c>
     </row>
   </sheetData>
@@ -1486,51 +1539,51 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>7</v>
+        <v>109</v>
       </c>
       <c r="B2">
         <v>141</v>
       </c>
       <c r="C2">
-        <v>0.61757947852345074</v>
+        <v>0.45686328503117302</v>
       </c>
       <c r="D2">
-        <v>0.77439736313219443</v>
+        <v>0.51434373358465868</v>
       </c>
       <c r="E2">
-        <v>0.87999850177838057</v>
+        <v>0.71717761648329392</v>
       </c>
       <c r="F2">
-        <v>0.29375517424362241</v>
+        <v>0.62991908018888965</v>
       </c>
     </row>
   </sheetData>
@@ -1539,51 +1592,51 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>141</v>
       </c>
       <c r="C2">
-        <v>0.41215703292356232</v>
+        <v>0.61757947852345074</v>
       </c>
       <c r="D2">
-        <v>0.50561412837917052</v>
+        <v>0.77439736313219443</v>
       </c>
       <c r="E2">
-        <v>0.71106548810863446</v>
+        <v>0.87999850177838057</v>
       </c>
       <c r="F2">
-        <v>0.37130059860186709</v>
+        <v>0.29375517424362241</v>
       </c>
     </row>
   </sheetData>
@@ -1592,51 +1645,51 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>120</v>
+        <v>16</v>
       </c>
       <c r="B2">
         <v>141</v>
       </c>
       <c r="C2">
-        <v>0.56093229907034836</v>
+        <v>0.41215703292356232</v>
       </c>
       <c r="D2">
-        <v>0.50911114893122045</v>
+        <v>0.50561412837917052</v>
       </c>
       <c r="E2">
-        <v>0.7135202512411406</v>
+        <v>0.71106548810863446</v>
       </c>
       <c r="F2">
-        <v>0.36695227325977542</v>
+        <v>0.37130059860186709</v>
       </c>
     </row>
   </sheetData>
@@ -1645,34 +1698,87 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>120</v>
+      </c>
+      <c r="B2">
+        <v>141</v>
+      </c>
+      <c r="C2">
+        <v>0.56093229907034836</v>
+      </c>
+      <c r="D2">
+        <v>0.50911114893122045</v>
+      </c>
+      <c r="E2">
+        <v>0.7135202512411406</v>
+      </c>
+      <c r="F2">
+        <v>0.36695227325977542</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>15</v>
       </c>
@@ -1704,11 +1810,11 @@
   </sheetPr>
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView zoomScale="117" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" customWidth="1"/>
@@ -1719,12 +1825,12 @@
     <col min="8" max="8" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>14</v>
       </c>
@@ -1747,7 +1853,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>20</v>
       </c>
@@ -1759,24 +1865,24 @@
         <f>arbolts!B2</f>
         <v>73</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <f>arbolts!E2</f>
         <v>0.69789306115382232</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <f>arbolts!C2</f>
         <v>0.53666201145534653</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="1">
         <f>arbolts!F2</f>
         <v>0.1796952182466954</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="1">
         <f>arbolts!D2</f>
         <v>0.48705472480665268</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>21</v>
       </c>
@@ -1788,24 +1894,24 @@
         <f>bosquets!B2</f>
         <v>141</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <f>bosquets!E2</f>
         <v>0.54923039688708331</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <f>bosquets!C2</f>
         <v>0.39007369697755317</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="1">
         <f>bosquets!F2</f>
         <v>0.28283245527651962</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="1">
         <f>bosquets!D2</f>
         <v>0.30165402886474307</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>22</v>
       </c>
@@ -1817,24 +1923,24 @@
         <f>knnts!B2</f>
         <v>141</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <f>knnts!E2</f>
         <v>0.58068985278576613</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1">
         <f>knnts!C2</f>
         <v>0.42100411351496547</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="1">
         <f>knnts!F2</f>
         <v>0.1983219893132574</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="1">
         <f>knnts!D2</f>
         <v>0.33720070512835471</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>23</v>
       </c>
@@ -1857,7 +1963,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>24</v>
       </c>
@@ -1869,24 +1975,24 @@
         <f>arboltd!B2</f>
         <v>141</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="1">
         <f>arboltd!E2</f>
         <v>0.76340252578882917</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="1">
         <f>arboltd!C2</f>
         <v>0.63715007475836971</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="1">
         <f>arboltd!F2</f>
         <v>6.0277174820504209E-2</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="1">
         <f>arboltd!D2</f>
         <v>0.58278341638076392</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>25</v>
       </c>
@@ -1898,24 +2004,24 @@
         <f>bosquetd!B2</f>
         <v>141</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="1">
         <f>bosquetd!E2</f>
         <v>0.60230538728987482</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="1">
         <f>bosquetd!C2</f>
         <v>0.46495027524808641</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="1">
         <f>bosquetd!F2</f>
         <v>0.41504011267320101</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="1">
         <f>bosquetd!D2</f>
         <v>0.36277177955840612</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>26</v>
       </c>
@@ -1927,24 +2033,24 @@
         <f>knntd!B2</f>
         <v>38</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="1">
         <f>knntd!E2</f>
         <v>0.88759293928733585</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="1">
         <f>knntd!C2</f>
         <v>0.73506707758920142</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="1">
         <f>knntd!F2</f>
         <v>0.21965296744774859</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="1">
         <f>knntd!D2</f>
         <v>0.78782122587273218</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>27</v>
       </c>
@@ -1967,7 +2073,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>28</v>
       </c>
@@ -1979,24 +2085,24 @@
         <f>arbolcc!B2</f>
         <v>141</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="1">
         <f>arbolcc!E2</f>
         <v>0.9126975926134302</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="1">
         <f>arbolcc!C2</f>
         <v>0.5954445053546944</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="1">
         <f>arbolcc!F2</f>
         <v>0.24029458225554121</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="1">
         <f>arbolcc!D2</f>
         <v>0.83301689556235092</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>29</v>
       </c>
@@ -2008,24 +2114,24 @@
         <f>bosquecc!B2</f>
         <v>141</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="1">
         <f>bosquecc!E2</f>
         <v>0.71717761648329392</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="1">
         <f>bosquecc!C2</f>
         <v>0.45686328503117302</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="1">
         <f>bosquecc!F2</f>
         <v>0.62991908018888965</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14" s="1">
         <f>bosquecc!D2</f>
         <v>0.51434373358465868</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>30</v>
       </c>
@@ -2037,24 +2143,24 @@
         <f>knncc!B2</f>
         <v>141</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="1">
         <f>knncc!E2</f>
         <v>0.87999850177838057</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="1">
         <f>knncc!C2</f>
         <v>0.61757947852345074</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="1">
         <f>knncc!F2</f>
         <v>0.29375517424362241</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="1">
         <f>knncc!D2</f>
         <v>0.77439736313219443</v>
       </c>
     </row>
-    <row r="17" spans="2:11">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>31</v>
       </c>
@@ -2077,7 +2183,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="2:11">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>32</v>
       </c>
@@ -2089,24 +2195,24 @@
         <f>arbolpp!B2</f>
         <v>141</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="1">
         <f>arbolpp!E2</f>
         <v>0.71106548810863446</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="1">
         <f>arbolpp!C2</f>
         <v>0.41215703292356232</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18" s="1">
         <f>arbolpp!F2</f>
         <v>0.37130059860186709</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18" s="1">
         <f>arbolpp!D2</f>
         <v>0.50561412837917052</v>
       </c>
     </row>
-    <row r="19" spans="2:11">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>33</v>
       </c>
@@ -2118,24 +2224,24 @@
         <f>bosquepp!B2</f>
         <v>141</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="1">
         <f>bosquepp!E2</f>
         <v>0.7135202512411406</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="1">
         <f>bosquepp!C2</f>
         <v>0.56093229907034836</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19" s="1">
         <f>bosquepp!F2</f>
         <v>0.36695227325977542</v>
       </c>
-      <c r="H19" s="2">
+      <c r="H19" s="1">
         <f>bosquepp!D2</f>
         <v>0.50911114893122045</v>
       </c>
     </row>
-    <row r="20" spans="2:11">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>34</v>
       </c>
@@ -2147,24 +2253,24 @@
         <f>knnpp!B2</f>
         <v>73</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="1">
         <f>knnpp!E2</f>
         <v>1.0379250862120271</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="1">
         <f>knnpp!C2</f>
         <v>0.74173940818638218</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20" s="1">
         <f>knnpp!F2</f>
         <v>0.17204262238063209</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H20" s="1">
         <f>knnpp!D2</f>
         <v>1.077288484588244</v>
       </c>
     </row>
-    <row r="22" spans="2:11">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>35</v>
       </c>
@@ -2196,7 +2302,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="2:11">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>11</v>
       </c>
@@ -2216,28 +2322,28 @@
         <f>arbolu!D2</f>
         <v>9.9980774776329134E-2</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G23" s="1">
         <f>arbolu!E2</f>
         <v>0.70588235294117652</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H23" s="1">
         <f>arbolu!F2</f>
         <v>0.66024340770791068</v>
       </c>
-      <c r="I23" s="2">
+      <c r="I23" s="1">
         <f>arbolu!G2</f>
         <v>0.70588235294117652</v>
       </c>
-      <c r="J23" s="2">
+      <c r="J23" s="1">
         <f>arbolu!H2</f>
         <v>0.6384803921568627</v>
       </c>
-      <c r="K23" s="2">
+      <c r="K23" s="1">
         <f>arbolu!I2</f>
         <v>0.82958477508650519</v>
       </c>
     </row>
-    <row r="24" spans="2:11">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>12</v>
       </c>
@@ -2257,28 +2363,28 @@
         <f>bosqueu!D2</f>
         <v>4.9990387388164567E-2</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G24" s="1">
         <f>bosqueu!E2</f>
         <v>0.67647058823529416</v>
       </c>
-      <c r="H24" s="2">
+      <c r="H24" s="1">
         <f>bosqueu!F2</f>
         <v>0.70053475935828879</v>
       </c>
-      <c r="I24" s="2">
+      <c r="I24" s="1">
         <f>bosqueu!G2</f>
         <v>0.67647058823529416</v>
       </c>
-      <c r="J24" s="2">
+      <c r="J24" s="1">
         <f>bosqueu!H2</f>
         <v>0.66654710664753702</v>
       </c>
-      <c r="K24" s="2">
+      <c r="K24" s="1">
         <f>bosqueu!I2</f>
         <v>0.87600922722029984</v>
       </c>
     </row>
-    <row r="25" spans="2:11">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>13</v>
       </c>
@@ -2298,23 +2404,23 @@
         <f>knnu!D2</f>
         <v>0</v>
       </c>
-      <c r="G25" s="2">
+      <c r="G25" s="1">
         <f>knnu!E2</f>
         <v>0.55882352941176472</v>
       </c>
-      <c r="H25" s="2">
+      <c r="H25" s="1">
         <f>knnu!F2</f>
         <v>0.31228373702422152</v>
       </c>
-      <c r="I25" s="2">
+      <c r="I25" s="1">
         <f>knnu!G2</f>
         <v>0.55882352941176472</v>
       </c>
-      <c r="J25" s="2">
+      <c r="J25" s="1">
         <f>knnu!H2</f>
         <v>0.40066592674805768</v>
       </c>
-      <c r="K25" s="2">
+      <c r="K25" s="1">
         <f>knnu!I2</f>
         <v>0.81660899653979235</v>
       </c>
@@ -2573,55 +2679,915 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200"/>
   <tableParts count="5">
+    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
-    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{666C0CE1-8A9B-4F75-A0AB-7D423F64C921}">
+  <dimension ref="C2:I35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B19" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" customWidth="1"/>
+    <col min="5" max="5" width="25" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>73</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.69789306115382232</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.53666201145534653</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0.1796952182466954</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0.48705472480665268</v>
+      </c>
+    </row>
+    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4">
+        <v>114</v>
+      </c>
+      <c r="E4">
+        <v>141</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.54923039688708331</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.39007369697755317</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.28283245527651962</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0.30165402886474307</v>
+      </c>
+    </row>
+    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5">
+        <v>17</v>
+      </c>
+      <c r="E5">
+        <v>141</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.58068985278576613</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.42100411351496547</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0.1983219893132574</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0.33720070512835471</v>
+      </c>
+    </row>
+    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7">
+        <v>16</v>
+      </c>
+      <c r="E7">
+        <v>141</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.76340252578882917</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.63715007475836971</v>
+      </c>
+      <c r="H7" s="1">
+        <v>6.0277174820504209E-2</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0.58278341638076392</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8">
+        <v>119</v>
+      </c>
+      <c r="E8">
+        <v>141</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.60230538728987482</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.46495027524808641</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0.41504011267320101</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0.36277177955840612</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9">
+        <v>7</v>
+      </c>
+      <c r="E9">
+        <v>38</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.88759293928733585</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.73506707758920142</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0.21965296744774859</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0.78782122587273218</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11">
+        <v>8</v>
+      </c>
+      <c r="E11">
+        <v>141</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0.9126975926134302</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.5954445053546944</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0.24029458225554121</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0.83301689556235092</v>
+      </c>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12">
+        <v>109</v>
+      </c>
+      <c r="E12">
+        <v>141</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.71717761648329392</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0.45686328503117302</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0.62991908018888965</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0.51434373358465868</v>
+      </c>
+    </row>
+    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13">
+        <v>7</v>
+      </c>
+      <c r="E13">
+        <v>141</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0.87999850177838057</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0.61757947852345074</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0.29375517424362241</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0.77439736313219443</v>
+      </c>
+    </row>
+    <row r="14" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15">
+        <v>16</v>
+      </c>
+      <c r="E15">
+        <v>141</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0.71106548810863446</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0.41215703292356232</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0.37130059860186709</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0.50561412837917052</v>
+      </c>
+    </row>
+    <row r="16" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16">
+        <v>120</v>
+      </c>
+      <c r="E16">
+        <v>141</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0.7135202512411406</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0.56093229907034836</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0.36695227325977542</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0.50911114893122045</v>
+      </c>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17">
+        <v>15</v>
+      </c>
+      <c r="E17">
+        <v>73</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1.0379250862120271</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0.74173940818638218</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0.17204262238063209</v>
+      </c>
+      <c r="I17" s="1">
+        <v>1.077288484588244</v>
+      </c>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" t="s">
+        <v>3</v>
+      </c>
+      <c r="F20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" t="s">
+        <v>18</v>
+      </c>
+      <c r="I20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21">
+        <v>73</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0.69789306115382232</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0.53666201145534653</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0.1796952182466954</v>
+      </c>
+      <c r="I21" s="1">
+        <v>0.48705472480665268</v>
+      </c>
+    </row>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22">
+        <v>114</v>
+      </c>
+      <c r="E22">
+        <v>141</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0.54923039688708331</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0.39007369697755317</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0.28283245527651962</v>
+      </c>
+      <c r="I22" s="1">
+        <v>0.30165402886474307</v>
+      </c>
+    </row>
+    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23">
+        <v>17</v>
+      </c>
+      <c r="E23">
+        <v>141</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0.58068985278576613</v>
+      </c>
+      <c r="G23" s="1">
+        <v>0.42100411351496547</v>
+      </c>
+      <c r="H23" s="1">
+        <v>0.1983219893132574</v>
+      </c>
+      <c r="I23" s="1">
+        <v>0.33720070512835471</v>
+      </c>
+    </row>
+    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" t="s">
+        <v>3</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25">
+        <v>16</v>
+      </c>
+      <c r="E25">
+        <v>141</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0.76340252578882917</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0.63715007475836971</v>
+      </c>
+      <c r="H25" s="1">
+        <v>6.0277174820504209E-2</v>
+      </c>
+      <c r="I25" s="1">
+        <v>0.58278341638076392</v>
+      </c>
+    </row>
+    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26">
+        <v>119</v>
+      </c>
+      <c r="E26">
+        <v>141</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0.60230538728987482</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0.46495027524808641</v>
+      </c>
+      <c r="H26" s="1">
+        <v>0.41504011267320101</v>
+      </c>
+      <c r="I26" s="1">
+        <v>0.36277177955840612</v>
+      </c>
+    </row>
+    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27">
+        <v>7</v>
+      </c>
+      <c r="E27">
+        <v>38</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0.88759293928733585</v>
+      </c>
+      <c r="G27" s="1">
+        <v>0.73506707758920142</v>
+      </c>
+      <c r="H27" s="1">
+        <v>0.21965296744774859</v>
+      </c>
+      <c r="I27" s="1">
+        <v>0.78782122587273218</v>
+      </c>
+    </row>
+    <row r="28" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" t="s">
+        <v>3</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29">
+        <v>8</v>
+      </c>
+      <c r="E29">
+        <v>141</v>
+      </c>
+      <c r="F29" s="1">
+        <v>0.9126975926134302</v>
+      </c>
+      <c r="G29" s="1">
+        <v>0.5954445053546944</v>
+      </c>
+      <c r="H29" s="1">
+        <v>0.24029458225554121</v>
+      </c>
+      <c r="I29" s="1">
+        <v>0.83301689556235092</v>
+      </c>
+    </row>
+    <row r="30" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30">
+        <v>109</v>
+      </c>
+      <c r="E30">
+        <v>141</v>
+      </c>
+      <c r="F30" s="1">
+        <v>0.71717761648329392</v>
+      </c>
+      <c r="G30" s="1">
+        <v>0.45686328503117302</v>
+      </c>
+      <c r="H30" s="1">
+        <v>0.62991908018888965</v>
+      </c>
+      <c r="I30" s="1">
+        <v>0.51434373358465868</v>
+      </c>
+    </row>
+    <row r="31" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31">
+        <v>7</v>
+      </c>
+      <c r="E31">
+        <v>141</v>
+      </c>
+      <c r="F31" s="1">
+        <v>0.87999850177838057</v>
+      </c>
+      <c r="G31" s="1">
+        <v>0.61757947852345074</v>
+      </c>
+      <c r="H31" s="1">
+        <v>0.29375517424362241</v>
+      </c>
+      <c r="I31" s="1">
+        <v>0.77439736313219443</v>
+      </c>
+    </row>
+    <row r="32" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E32" t="s">
+        <v>3</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33">
+        <v>16</v>
+      </c>
+      <c r="E33">
+        <v>141</v>
+      </c>
+      <c r="F33" s="1">
+        <v>0.71106548810863446</v>
+      </c>
+      <c r="G33" s="1">
+        <v>0.41215703292356232</v>
+      </c>
+      <c r="H33" s="1">
+        <v>0.37130059860186709</v>
+      </c>
+      <c r="I33" s="1">
+        <v>0.50561412837917052</v>
+      </c>
+    </row>
+    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34">
+        <v>120</v>
+      </c>
+      <c r="E34">
+        <v>141</v>
+      </c>
+      <c r="F34" s="1">
+        <v>0.7135202512411406</v>
+      </c>
+      <c r="G34" s="1">
+        <v>0.56093229907034836</v>
+      </c>
+      <c r="H34" s="1">
+        <v>0.36695227325977542</v>
+      </c>
+      <c r="I34" s="1">
+        <v>0.50911114893122045</v>
+      </c>
+    </row>
+    <row r="35" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35">
+        <v>15</v>
+      </c>
+      <c r="E35">
+        <v>73</v>
+      </c>
+      <c r="F35" s="1">
+        <v>1.0379250862120271</v>
+      </c>
+      <c r="G35" s="1">
+        <v>0.74173940818638218</v>
+      </c>
+      <c r="H35" s="1">
+        <v>0.17204262238063209</v>
+      </c>
+      <c r="I35" s="1">
+        <v>1.077288484588244</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="G3:G17">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F17">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:H17">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3:I17">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F22 F26 F30 F34">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G26 G22 G30 G34">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H22 H26 H30 H34">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I26 I22 I30 I34">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>4</v>
       </c>
@@ -2648,79 +3614,6 @@
       </c>
       <c r="I2">
         <v>0.82958477508650519</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:I2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2">
-        <v>111</v>
-      </c>
-      <c r="B2">
-        <v>73</v>
-      </c>
-      <c r="C2">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="D2">
-        <v>4.9990387388164567E-2</v>
-      </c>
-      <c r="E2">
-        <v>0.67647058823529416</v>
-      </c>
-      <c r="F2">
-        <v>0.70053475935828879</v>
-      </c>
-      <c r="G2">
-        <v>0.67647058823529416</v>
-      </c>
-      <c r="H2">
-        <v>0.66654710664753702</v>
-      </c>
-      <c r="I2">
-        <v>0.87600922722029984</v>
       </c>
     </row>
   </sheetData>
@@ -2729,69 +3622,69 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>23</v>
+        <v>111</v>
       </c>
       <c r="B2">
-        <v>38</v>
+        <v>73</v>
       </c>
       <c r="C2">
-        <v>0.55882352941176472</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>4.9990387388164567E-2</v>
       </c>
       <c r="E2">
-        <v>0.55882352941176472</v>
+        <v>0.67647058823529416</v>
       </c>
       <c r="F2">
-        <v>0.31228373702422152</v>
+        <v>0.70053475935828879</v>
       </c>
       <c r="G2">
-        <v>0.55882352941176472</v>
+        <v>0.67647058823529416</v>
       </c>
       <c r="H2">
-        <v>0.40066592674805768</v>
+        <v>0.66654710664753702</v>
       </c>
       <c r="I2">
-        <v>0.81660899653979235</v>
+        <v>0.87600922722029984</v>
       </c>
     </row>
   </sheetData>
@@ -2800,59 +3693,69 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="B2">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="C2">
-        <v>0.53666201145534653</v>
+        <v>0.55882352941176472</v>
       </c>
       <c r="D2">
-        <v>0.48705472480665268</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>0.69789306115382232</v>
+        <v>0.55882352941176472</v>
       </c>
       <c r="F2">
-        <v>0.1796952182466954</v>
+        <v>0.31228373702422152</v>
+      </c>
+      <c r="G2">
+        <v>0.55882352941176472</v>
+      </c>
+      <c r="H2">
+        <v>0.40066592674805768</v>
+      </c>
+      <c r="I2">
+        <v>0.81660899653979235</v>
       </c>
     </row>
   </sheetData>
@@ -2861,60 +3764,51 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2">
         <v>73</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2">
-        <v>114</v>
-      </c>
-      <c r="B2">
-        <v>141</v>
-      </c>
       <c r="C2">
-        <v>0.39007369697755317</v>
+        <v>0.53666201145534653</v>
       </c>
       <c r="D2">
-        <v>0.30165402886474307</v>
+        <v>0.48705472480665268</v>
       </c>
       <c r="E2">
-        <v>0.54923039688708331</v>
+        <v>0.69789306115382232</v>
       </c>
       <c r="F2">
-        <v>0.28283245527651962</v>
+        <v>0.1796952182466954</v>
       </c>
     </row>
   </sheetData>
@@ -2923,53 +3817,51 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>17</v>
+        <v>114</v>
       </c>
       <c r="B2">
         <v>141</v>
       </c>
       <c r="C2">
-        <v>0.42100411351496547</v>
+        <v>0.39007369697755317</v>
       </c>
       <c r="D2">
-        <v>0.33720070512835471</v>
+        <v>0.30165402886474307</v>
       </c>
       <c r="E2">
-        <v>0.58068985278576613</v>
+        <v>0.54923039688708331</v>
       </c>
       <c r="F2">
-        <v>0.1983219893132574</v>
+        <v>0.28283245527651962</v>
       </c>
     </row>
   </sheetData>
@@ -2978,51 +3870,51 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2">
         <v>141</v>
       </c>
       <c r="C2">
-        <v>0.63715007475836971</v>
+        <v>0.42100411351496547</v>
       </c>
       <c r="D2">
-        <v>0.58278341638076392</v>
+        <v>0.33720070512835471</v>
       </c>
       <c r="E2">
-        <v>0.76340252578882917</v>
+        <v>0.58068985278576613</v>
       </c>
       <c r="F2">
-        <v>6.0277174820504209E-2</v>
+        <v>0.1983219893132574</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
buscando la forma de crear un solo y_prueba para comparar los resultados
</commit_message>
<xml_diff>
--- a/resultadospython.xlsx
+++ b/resultadospython.xlsx
@@ -997,16 +997,16 @@
         <v>141</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4628680854612942</v>
+        <v>0.4649502752480864</v>
       </c>
       <c r="D2" t="n">
-        <v>0.3603959740228815</v>
+        <v>0.3627717795584061</v>
       </c>
       <c r="E2" t="n">
-        <v>0.6003298876641755</v>
+        <v>0.6023053872898748</v>
       </c>
       <c r="F2" t="n">
-        <v>0.4188710361812604</v>
+        <v>0.415040112673201</v>
       </c>
     </row>
   </sheetData>
@@ -2850,13 +2850,13 @@
         <v>0.5366620114553465</v>
       </c>
       <c r="D2" t="n">
-        <v>0.4870547248066529</v>
+        <v>0.4870547248066527</v>
       </c>
       <c r="E2" t="n">
         <v>0.6978930611538223</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1796952182466958</v>
+        <v>0.1796952182466954</v>
       </c>
     </row>
   </sheetData>
@@ -2918,16 +2918,16 @@
         <v>141</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3868215117320903</v>
+        <v>0.3900736969775532</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2953342089682264</v>
+        <v>0.3016540288647431</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5434466017634358</v>
+        <v>0.5492303968870833</v>
       </c>
       <c r="F2" t="n">
-        <v>0.2978575147306793</v>
+        <v>0.2828324552765196</v>
       </c>
     </row>
   </sheetData>
@@ -2989,16 +2989,16 @@
         <v>141</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4210041135149656</v>
+        <v>0.4210041135149655</v>
       </c>
       <c r="D2" t="n">
-        <v>0.3372007051283548</v>
+        <v>0.3372007051283547</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5806898527857662</v>
+        <v>0.5806898527857661</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1983219893132575</v>
+        <v>0.1983219893132574</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bosqueu finalizado con un solo arreglo aleatorio
</commit_message>
<xml_diff>
--- a/resultadospython.xlsx
+++ b/resultadospython.xlsx
@@ -2514,7 +2514,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2525,45 +2525,30 @@
     <row r="1">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>Profundidad óptima arbolu</t>
+          <t>Profundidad óptima</t>
         </is>
       </c>
       <c r="B1" s="3" t="inlineStr">
         <is>
-          <t>Arreglo aleatorio óptimo arbolu</t>
+          <t>Exactitud arbolu</t>
         </is>
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>Exactitud media arbolu</t>
+          <t>Precisión arbolu</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
         <is>
-          <t>Desviación estándar de la exactitud arbolu</t>
+          <t>Sensibilidad arbolu</t>
         </is>
       </c>
       <c r="E1" s="3" t="inlineStr">
         <is>
-          <t>Exactitud arbolu</t>
+          <t>Puntaje F1 arbolu</t>
         </is>
       </c>
       <c r="F1" s="3" t="inlineStr">
-        <is>
-          <t>Precisión arbolu</t>
-        </is>
-      </c>
-      <c r="G1" s="3" t="inlineStr">
-        <is>
-          <t>Sensibilidad arbolu</t>
-        </is>
-      </c>
-      <c r="H1" s="3" t="inlineStr">
-        <is>
-          <t>F1-score arbolu</t>
-        </is>
-      </c>
-      <c r="I1" s="3" t="inlineStr">
         <is>
           <t>ROC/AUC arbolu</t>
         </is>
@@ -2574,27 +2559,18 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>38</v>
+        <v>0.7058823529411765</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5686274509803922</v>
+        <v>0.6602434077079107</v>
       </c>
       <c r="D2" t="n">
-        <v>0.09998077477632913</v>
+        <v>0.7058823529411765</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7058823529411765</v>
+        <v>0.6384803921568627</v>
       </c>
       <c r="F2" t="n">
-        <v>0.6602434077079107</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.7058823529411765</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.6384803921568627</v>
-      </c>
-      <c r="I2" t="n">
         <v>0.8295847750865052</v>
       </c>
     </row>
@@ -2609,7 +2585,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2620,45 +2596,30 @@
     <row r="1">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>Estimador óptimo bosqueu</t>
+          <t>Estimador óptimo</t>
         </is>
       </c>
       <c r="B1" s="3" t="inlineStr">
         <is>
-          <t>Arreglo aleatorio óptimo bosqueu</t>
+          <t>Exactitud bosqueu</t>
         </is>
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>Exactitud media bosqueu</t>
+          <t>Precisión bosqueu</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
         <is>
-          <t>Desviación estándar de la exactitud bosqueu</t>
+          <t>Sensibilidad bosqueu</t>
         </is>
       </c>
       <c r="E1" s="3" t="inlineStr">
         <is>
-          <t>Exactitud bosqueu</t>
+          <t>Puntaje F1 bosqueu</t>
         </is>
       </c>
       <c r="F1" s="3" t="inlineStr">
-        <is>
-          <t>Precisión bosqueu</t>
-        </is>
-      </c>
-      <c r="G1" s="3" t="inlineStr">
-        <is>
-          <t>Sensibilidad bosqueu</t>
-        </is>
-      </c>
-      <c r="H1" s="3" t="inlineStr">
-        <is>
-          <t>F1-score bosqueu</t>
-        </is>
-      </c>
-      <c r="I1" s="3" t="inlineStr">
         <is>
           <t>ROC/AUC bosqueu</t>
         </is>
@@ -2666,31 +2627,22 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B2" t="n">
-        <v>73</v>
+        <v>0.6470588235294118</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.6366223908918406</v>
       </c>
       <c r="D2" t="n">
-        <v>0.04999038738816457</v>
+        <v>0.6470588235294118</v>
       </c>
       <c r="E2" t="n">
-        <v>0.6764705882352942</v>
+        <v>0.5604524886877827</v>
       </c>
       <c r="F2" t="n">
-        <v>0.7005347593582888</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.6764705882352942</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.666547106647537</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.8760092272202998</v>
+        <v>0.8468858131487889</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1. voy con knn de tension sistolica; 2. agregare las pruebas MAE, MSE, RMSE y R2 a las definiciones del codigo; 3. tambien falta ver cual prueba recomienda el libro para hacerle igual que en el libro
</commit_message>
<xml_diff>
--- a/resultadospython.xlsx
+++ b/resultadospython.xlsx
@@ -2814,7 +2814,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2825,53 +2825,45 @@
     <row r="1">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>Estimador óptimo bosquets</t>
+          <t>Estimador óptimo</t>
         </is>
       </c>
       <c r="B1" s="3" t="inlineStr">
         <is>
-          <t>Arreglo aleatorio óptimo bosquets</t>
+          <t>MAE bosquets</t>
         </is>
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>MAE bosquets</t>
+          <t>MSE bosquets</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
         <is>
-          <t>MSE bosquets</t>
+          <t>RMSE bosquets</t>
         </is>
       </c>
       <c r="E1" s="3" t="inlineStr">
         <is>
-          <t>RMSE bosquets</t>
-        </is>
-      </c>
-      <c r="F1" s="3" t="inlineStr">
-        <is>
-          <t>R-cuadrado bosquets</t>
+          <t>R2 bosquets</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="B2" t="n">
-        <v>141</v>
+        <v>0.6082810349699448</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3918569649202684</v>
+        <v>0.5844243957844734</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2983586230873764</v>
+        <v>0.7644765501861214</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5462221371268071</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.2906671196405792</v>
+        <v>0.03229832537117805</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1. termine la eleccion del mejor modelo para tensió sistólica; 2. tengo que ver que son los cell tags; 3. ver si se puede ver el significado o el resultado de las variables al poner encima el curso; 4. agregar mae, mse, rmse y r2 a las definiciones del codigo; 5. ver cual prueba recomeinda el libro
</commit_message>
<xml_diff>
--- a/resultadospython.xlsx
+++ b/resultadospython.xlsx
@@ -2877,7 +2877,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2888,53 +2888,45 @@
     <row r="1">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>K óptimo knnts</t>
+          <t>K óptimo</t>
         </is>
       </c>
       <c r="B1" s="3" t="inlineStr">
         <is>
-          <t>Arreglo aleatorio óptimo knnts</t>
+          <t>MAE knnts</t>
         </is>
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>MAE knnts</t>
+          <t>MSE knnts</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
         <is>
-          <t>MSE knnts</t>
+          <t>RMSE knnts</t>
         </is>
       </c>
       <c r="E1" s="3" t="inlineStr">
         <is>
-          <t>RMSE knnts</t>
-        </is>
-      </c>
-      <c r="F1" s="3" t="inlineStr">
-        <is>
-          <t>R-cuadrado knnts</t>
+          <t>R2 knnts</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B2" t="n">
-        <v>141</v>
+        <v>0.5753903495649837</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4491258397360403</v>
+        <v>0.6224774416917598</v>
       </c>
       <c r="D2" t="n">
-        <v>0.3373863112421027</v>
+        <v>0.7889723960264768</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5808496459860354</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.1978807199511898</v>
+        <v>-0.03071067376510817</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
inicio PLOTS con Seaborn, inicio con modelots
</commit_message>
<xml_diff>
--- a/resultadospython.xlsx
+++ b/resultadospython.xlsx
@@ -991,22 +991,22 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B2" t="n">
         <v>141</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4620667186862082</v>
+        <v>0.4403635287824023</v>
       </c>
       <c r="D2" t="n">
-        <v>0.3795576163023952</v>
+        <v>0.3445842163252649</v>
       </c>
       <c r="E2" t="n">
-        <v>0.6160824752436926</v>
+        <v>0.5870129609516853</v>
       </c>
       <c r="F2" t="n">
-        <v>0.3879733954594133</v>
+        <v>0.4443670767291096</v>
       </c>
     </row>
   </sheetData>
@@ -1062,22 +1062,22 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B2" t="n">
-        <v>73</v>
+        <v>141</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5052149582680001</v>
+        <v>0.5163314425842619</v>
       </c>
       <c r="D2" t="n">
-        <v>0.4451703388478029</v>
+        <v>0.5053587189483683</v>
       </c>
       <c r="E2" t="n">
-        <v>0.6672108653550262</v>
+        <v>0.7108858691438227</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1856922731716195</v>
+        <v>0.1851224490077538</v>
       </c>
     </row>
   </sheetData>
@@ -1133,22 +1133,22 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B2" t="n">
-        <v>141</v>
+        <v>73</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5127502274240259</v>
+        <v>0.5224162527917269</v>
       </c>
       <c r="D2" t="n">
-        <v>0.6261282584550604</v>
+        <v>0.5561315165518705</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7912826665958634</v>
+        <v>0.7457422587944649</v>
       </c>
       <c r="F2" t="n">
-        <v>0.4289755313665086</v>
+        <v>0.2214155788200853</v>
       </c>
     </row>
   </sheetData>
@@ -1204,22 +1204,22 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B2" t="n">
         <v>141</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4538677131172378</v>
+        <v>0.465431751554182</v>
       </c>
       <c r="D2" t="n">
-        <v>0.508338953300392</v>
+        <v>0.5685521201615351</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7129789290718149</v>
+        <v>0.7540239519813248</v>
       </c>
       <c r="F2" t="n">
-        <v>0.6342396433954777</v>
+        <v>0.5909150285092269</v>
       </c>
     </row>
   </sheetData>
@@ -1275,22 +1275,22 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B2" t="n">
         <v>141</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6175794785234507</v>
+        <v>0.6839272017166228</v>
       </c>
       <c r="D2" t="n">
-        <v>0.7743973631321944</v>
+        <v>0.9553986818988459</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8799985017783806</v>
+        <v>0.9774449764047314</v>
       </c>
       <c r="F2" t="n">
-        <v>0.2937551742436224</v>
+        <v>0.1286832732792506</v>
       </c>
     </row>
   </sheetData>
@@ -1346,22 +1346,22 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B2" t="n">
-        <v>141</v>
+        <v>38</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4121570329235623</v>
+        <v>0.5679002795599084</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5056141283791705</v>
+        <v>0.764300989333502</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7110654881086345</v>
+        <v>0.8742430951019871</v>
       </c>
       <c r="F2" t="n">
-        <v>0.3713005986018671</v>
+        <v>0.1299771267529172</v>
       </c>
     </row>
   </sheetData>
@@ -1417,22 +1417,22 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="B2" t="n">
         <v>141</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5579714008453226</v>
+        <v>0.5524929388862618</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5038784557938416</v>
+        <v>0.5280812406997041</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7098439658078679</v>
+        <v>0.7266919847498692</v>
       </c>
       <c r="F2" t="n">
-        <v>0.373458798411112</v>
+        <v>0.3433641560179854</v>
       </c>
     </row>
   </sheetData>
@@ -1488,22 +1488,22 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B2" t="n">
         <v>73</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7417394081863822</v>
+        <v>0.7410072360200077</v>
       </c>
       <c r="D2" t="n">
-        <v>1.077288484588244</v>
+        <v>1.109972397053677</v>
       </c>
       <c r="E2" t="n">
-        <v>1.037925086212027</v>
+        <v>1.053552275425229</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1720426223806321</v>
+        <v>0.1469231795922281</v>
       </c>
     </row>
   </sheetData>
@@ -2982,22 +2982,22 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B2" t="n">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6564576527813506</v>
+        <v>0.8173541363061914</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5972805162907332</v>
+        <v>1.066986553373737</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7728392564374129</v>
+        <v>1.032950411865805</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.09254839565102091</v>
+        <v>-0.05686387133831139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
decubriendo como funciona train_test_split
</commit_message>
<xml_diff>
--- a/resultadospython.xlsx
+++ b/resultadospython.xlsx
@@ -2791,16 +2791,16 @@
         <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>0.8561259825882406</v>
+        <v>0.6977341098772637</v>
       </c>
       <c r="C2" t="n">
-        <v>1.057866115220892</v>
+        <v>0.8658933832837197</v>
       </c>
       <c r="D2" t="n">
-        <v>1.028526185967519</v>
+        <v>0.9305339237683491</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.751636000509923</v>
+        <v>-1.732651912978245</v>
       </c>
     </row>
   </sheetData>
@@ -2851,19 +2851,19 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B2" t="n">
-        <v>0.6082810349699448</v>
+        <v>0.5045252397713184</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5844243957844734</v>
+        <v>0.484406475399015</v>
       </c>
       <c r="D2" t="n">
-        <v>0.7644765501861214</v>
+        <v>0.6959931575806008</v>
       </c>
       <c r="E2" t="n">
-        <v>0.03229832537117805</v>
+        <v>-0.5287266391137646</v>
       </c>
     </row>
   </sheetData>
@@ -2914,19 +2914,19 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B2" t="n">
-        <v>0.5753903495649837</v>
+        <v>0.4302434103874868</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6224774416917598</v>
+        <v>0.3679452024441739</v>
       </c>
       <c r="D2" t="n">
-        <v>0.7889723960264768</v>
+        <v>0.6065848682947621</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.03071067376510817</v>
+        <v>-0.1611893343233775</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se logra realizar los modelos, quitando la varibale pp y despues imputandola. ahora falta arreglar porque edad se modifico
</commit_message>
<xml_diff>
--- a/resultadospython.xlsx
+++ b/resultadospython.xlsx
@@ -2791,16 +2791,16 @@
         <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>0.6977341098772637</v>
+        <v>11.74729444162726</v>
       </c>
       <c r="C2" t="n">
-        <v>0.8658933832837197</v>
+        <v>270.5656953227698</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9305339237683491</v>
+        <v>16.44888127876087</v>
       </c>
       <c r="E2" t="n">
-        <v>-1.732651912978245</v>
+        <v>0.8726742175255467</v>
       </c>
     </row>
   </sheetData>
@@ -2851,19 +2851,19 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B2" t="n">
-        <v>0.5045252397713184</v>
+        <v>8.779559828778744</v>
       </c>
       <c r="C2" t="n">
-        <v>0.484406475399015</v>
+        <v>142.8535896048408</v>
       </c>
       <c r="D2" t="n">
-        <v>0.6959931575806008</v>
+        <v>11.95213744921137</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.5287266391137646</v>
+        <v>0.9327743857031751</v>
       </c>
     </row>
   </sheetData>
@@ -2914,19 +2914,19 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B2" t="n">
-        <v>0.4302434103874868</v>
+        <v>9.068932712817771</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3679452024441739</v>
+        <v>156.0077977761895</v>
       </c>
       <c r="D2" t="n">
-        <v>0.6065848682947621</v>
+        <v>12.49030815377225</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.1611893343233775</v>
+        <v>0.9265841336601331</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
arregle lo de retirar la variable pp, pero el arbol de decision sale mal en ts. lo que sigue es arreglarlo, despues cambiar lo de variable pp en los demas algoritmos de las otras variables y despues graficar
</commit_message>
<xml_diff>
--- a/resultadospython.xlsx
+++ b/resultadospython.xlsx
@@ -2556,22 +2556,22 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>0.7058823529411765</v>
+        <v>0.6121212121212121</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6602434077079107</v>
+        <v>0.4119706380575945</v>
       </c>
       <c r="D2" t="n">
-        <v>0.7058823529411765</v>
+        <v>0.6121212121212121</v>
       </c>
       <c r="E2" t="n">
-        <v>0.6384803921568627</v>
+        <v>0.4826078971533517</v>
       </c>
       <c r="F2" t="n">
-        <v>0.8295847750865052</v>
+        <v>0.7741169268441995</v>
       </c>
     </row>
   </sheetData>
@@ -2627,22 +2627,22 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B2" t="n">
-        <v>0.6470588235294118</v>
+        <v>0.6060606060606061</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6366223908918406</v>
+        <v>0.5653433616742969</v>
       </c>
       <c r="D2" t="n">
-        <v>0.6470588235294118</v>
+        <v>0.6060606060606061</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5604524886877827</v>
+        <v>0.542436518809878</v>
       </c>
       <c r="F2" t="n">
-        <v>0.847318339100346</v>
+        <v>0.771043771043771</v>
       </c>
     </row>
   </sheetData>
@@ -2791,16 +2791,16 @@
         <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>11.74729444162726</v>
+        <v>0.8708212942316997</v>
       </c>
       <c r="C2" t="n">
-        <v>270.5656953227698</v>
+        <v>1.385562392002157</v>
       </c>
       <c r="D2" t="n">
-        <v>16.44888127876087</v>
+        <v>1.177099142809201</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8726742175255467</v>
+        <v>-0.6717157196487737</v>
       </c>
     </row>
   </sheetData>
@@ -2851,19 +2851,19 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>102</v>
+        <v>124</v>
       </c>
       <c r="B2" t="n">
-        <v>8.779559828778744</v>
+        <v>0.6290313206092344</v>
       </c>
       <c r="C2" t="n">
-        <v>142.8535896048408</v>
+        <v>0.6401813750093149</v>
       </c>
       <c r="D2" t="n">
-        <v>11.95213744921137</v>
+        <v>0.8001133513504914</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9327743857031751</v>
+        <v>0.2276051412719259</v>
       </c>
     </row>
   </sheetData>
@@ -2914,19 +2914,19 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B2" t="n">
-        <v>9.068932712817771</v>
+        <v>0.6465181857472143</v>
       </c>
       <c r="C2" t="n">
-        <v>156.0077977761895</v>
+        <v>0.7076411505920056</v>
       </c>
       <c r="D2" t="n">
-        <v>12.49030815377225</v>
+        <v>0.8412140931962597</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9265841336601331</v>
+        <v>0.1462132328768061</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
vamos en circunferencia de cintura, con graficas de variables caterocias y de numericas hasta tension diastolica
</commit_message>
<xml_diff>
--- a/resultadospython.xlsx
+++ b/resultadospython.xlsx
@@ -949,7 +949,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -960,53 +960,45 @@
     <row r="1">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>Estimador óptimo bosquetd</t>
+          <t>Estimador óptimo</t>
         </is>
       </c>
       <c r="B1" s="3" t="inlineStr">
         <is>
-          <t>Arreglo aleatorio óptimo bosquetd</t>
+          <t>MAE bosquetd</t>
         </is>
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>MAE bosquetd</t>
+          <t>MSE bosquetd</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
         <is>
-          <t>MSE bosquetd</t>
+          <t>RMSE bosquetd</t>
         </is>
       </c>
       <c r="E1" s="3" t="inlineStr">
         <is>
-          <t>RMSE bosquetd</t>
-        </is>
-      </c>
-      <c r="F1" s="3" t="inlineStr">
-        <is>
-          <t>R-cuadrado bosquetd</t>
+          <t>R2 bosquetd</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="B2" t="n">
-        <v>141</v>
+        <v>0.4573004169495208</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4403635287824023</v>
+        <v>0.410033964531995</v>
       </c>
       <c r="D2" t="n">
-        <v>0.3445842163252649</v>
+        <v>0.6403389450377004</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5870129609516853</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.4443670767291096</v>
+        <v>0.6226367865212324</v>
       </c>
     </row>
   </sheetData>
@@ -1020,7 +1012,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1031,53 +1023,45 @@
     <row r="1">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>K óptimo knntd</t>
+          <t>K óptimo</t>
         </is>
       </c>
       <c r="B1" s="3" t="inlineStr">
         <is>
-          <t>Arreglo aleatorio óptimo knntd</t>
+          <t>MAE knntd</t>
         </is>
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>MAE knntd</t>
+          <t>MSE knntd</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
         <is>
-          <t>MSE knntd</t>
+          <t>RMSE knntd</t>
         </is>
       </c>
       <c r="E1" s="3" t="inlineStr">
         <is>
-          <t>RMSE knntd</t>
-        </is>
-      </c>
-      <c r="F1" s="3" t="inlineStr">
-        <is>
-          <t>R-cuadrado knntd</t>
+          <t>R2 knntd</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B2" t="n">
-        <v>141</v>
+        <v>0.6220102972122369</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5163314425842619</v>
+        <v>0.6818153889718599</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5053587189483683</v>
+        <v>0.8257211326906075</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7108858691438227</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.1851224490077538</v>
+        <v>0.3725104053871119</v>
       </c>
     </row>
   </sheetData>
@@ -2940,7 +2924,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2951,53 +2935,45 @@
     <row r="1">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>Profundidad óptima arboltd</t>
+          <t>Profundidad óptima</t>
         </is>
       </c>
       <c r="B1" s="3" t="inlineStr">
         <is>
-          <t>Arreglo aleatorio óptimo arboltd</t>
+          <t>MAE arboltd</t>
         </is>
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>MAE arboltd</t>
+          <t>MSE arboltd</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
         <is>
-          <t>MSE arboltd</t>
+          <t>RMSE arboltd</t>
         </is>
       </c>
       <c r="E1" s="3" t="inlineStr">
         <is>
-          <t>RMSE arboltd</t>
-        </is>
-      </c>
-      <c r="F1" s="3" t="inlineStr">
-        <is>
-          <t>R-cuadrado arboltd</t>
+          <t>R2 arboltd</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>38</v>
+        <v>0.6845854597204523</v>
       </c>
       <c r="C2" t="n">
-        <v>0.8173541363061914</v>
+        <v>0.7617854841998375</v>
       </c>
       <c r="D2" t="n">
-        <v>1.066986553373737</v>
+        <v>0.8728032333807189</v>
       </c>
       <c r="E2" t="n">
-        <v>1.032950411865805</v>
-      </c>
-      <c r="F2" t="n">
-        <v>-0.05686387133831139</v>
+        <v>0.2989121800501523</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ya esta el modelo completo con graficas. ahora voy a arreglar el articulo final
</commit_message>
<xml_diff>
--- a/resultadospython.xlsx
+++ b/resultadospython.xlsx
@@ -1075,7 +1075,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1086,53 +1086,45 @@
     <row r="1">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>Profundidad óptima arbolcc</t>
+          <t>Profundidad óptima</t>
         </is>
       </c>
       <c r="B1" s="3" t="inlineStr">
         <is>
-          <t>Arreglo aleatorio óptimo arbolcc</t>
+          <t>MAE arbolcc</t>
         </is>
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>MAE arbolcc</t>
+          <t>MSE arbolcc</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
         <is>
-          <t>MSE arbolcc</t>
+          <t>RMSE arbolcc</t>
         </is>
       </c>
       <c r="E1" s="3" t="inlineStr">
         <is>
-          <t>RMSE arbolcc</t>
-        </is>
-      </c>
-      <c r="F1" s="3" t="inlineStr">
-        <is>
-          <t>R-cuadrado arbolcc</t>
+          <t>R2 arbolcc</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>73</v>
+        <v>0.5774729620742622</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5224162527917269</v>
+        <v>0.6466338346268923</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5561315165518705</v>
+        <v>0.8041354578843618</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7457422587944649</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.2214155788200853</v>
+        <v>0.3648838465338654</v>
       </c>
     </row>
   </sheetData>
@@ -1146,7 +1138,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1157,53 +1149,45 @@
     <row r="1">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>Estimador óptimo bosquecc</t>
+          <t>Estimador óptimo</t>
         </is>
       </c>
       <c r="B1" s="3" t="inlineStr">
         <is>
-          <t>Arreglo aleatorio óptimo bosquecc</t>
+          <t>MAE bosquecc</t>
         </is>
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>MAE bosquecc</t>
+          <t>MSE bosquecc</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
         <is>
-          <t>MSE bosquecc</t>
+          <t>RMSE bosquecc</t>
         </is>
       </c>
       <c r="E1" s="3" t="inlineStr">
         <is>
-          <t>RMSE bosquecc</t>
-        </is>
-      </c>
-      <c r="F1" s="3" t="inlineStr">
-        <is>
-          <t>R-cuadrado bosquecc</t>
+          <t>R2 bosquecc</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B2" t="n">
-        <v>141</v>
+        <v>0.4293526781499747</v>
       </c>
       <c r="C2" t="n">
-        <v>0.465431751554182</v>
+        <v>0.3504596228933595</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5685521201615351</v>
+        <v>0.5919963031078483</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7540239519813248</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.5909150285092269</v>
+        <v>0.6557826768132963</v>
       </c>
     </row>
   </sheetData>
@@ -1217,7 +1201,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1228,32 +1212,27 @@
     <row r="1">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>K óptimo knncc</t>
+          <t>K óptimo</t>
         </is>
       </c>
       <c r="B1" s="3" t="inlineStr">
         <is>
-          <t>Arreglo aleatorio óptimo knncc</t>
+          <t>MAE knncc</t>
         </is>
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>MAE knncc</t>
+          <t>MSE knncc</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
         <is>
-          <t>MSE knncc</t>
+          <t>RMSE knncc</t>
         </is>
       </c>
       <c r="E1" s="3" t="inlineStr">
         <is>
-          <t>RMSE knncc</t>
-        </is>
-      </c>
-      <c r="F1" s="3" t="inlineStr">
-        <is>
-          <t>R-cuadrado knncc</t>
+          <t>R2 knncc</t>
         </is>
       </c>
     </row>
@@ -1262,19 +1241,16 @@
         <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>141</v>
+        <v>0.5326407001766574</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6839272017166228</v>
+        <v>0.4800962164278529</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9553986818988459</v>
+        <v>0.6928897577738128</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9774449764047314</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.1286832732792506</v>
+        <v>0.5284551380655178</v>
       </c>
     </row>
   </sheetData>
@@ -1288,7 +1264,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1299,53 +1275,45 @@
     <row r="1">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>Profundidad óptima arbolpp</t>
+          <t>Profundidad óptima</t>
         </is>
       </c>
       <c r="B1" s="3" t="inlineStr">
         <is>
-          <t>Arreglo aleatorio óptimo arbolpp</t>
+          <t>MAE arbolpp</t>
         </is>
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>MAE arbolpp</t>
+          <t>MSE arbolpp</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
         <is>
-          <t>MSE arbolpp</t>
+          <t>RMSE arbolpp</t>
         </is>
       </c>
       <c r="E1" s="3" t="inlineStr">
         <is>
-          <t>RMSE arbolpp</t>
-        </is>
-      </c>
-      <c r="F1" s="3" t="inlineStr">
-        <is>
-          <t>R-cuadrado arbolpp</t>
+          <t>R2 arbolpp</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="B2" t="n">
-        <v>38</v>
+        <v>0.775569221353989</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5679002795599084</v>
+        <v>1.827375618630338</v>
       </c>
       <c r="D2" t="n">
-        <v>0.764300989333502</v>
+        <v>1.351804578565385</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8742430951019871</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.1299771267529172</v>
+        <v>-1.115941009930692</v>
       </c>
     </row>
   </sheetData>
@@ -1359,7 +1327,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1370,53 +1338,45 @@
     <row r="1">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>Estimador óptimo bosquepp</t>
+          <t>Estimador óptimo</t>
         </is>
       </c>
       <c r="B1" s="3" t="inlineStr">
         <is>
-          <t>Arreglo aleatorio óptimo bosquepp</t>
+          <t>MAE bosquepp</t>
         </is>
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>MAE bosquepp</t>
+          <t>MSE bosquepp</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
         <is>
-          <t>MSE bosquepp</t>
+          <t>RMSE bosquepp</t>
         </is>
       </c>
       <c r="E1" s="3" t="inlineStr">
         <is>
-          <t>RMSE bosquepp</t>
-        </is>
-      </c>
-      <c r="F1" s="3" t="inlineStr">
-        <is>
-          <t>R-cuadrado bosquepp</t>
+          <t>R2 bosquepp</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B2" t="n">
-        <v>141</v>
+        <v>0.6276056324687056</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5524929388862618</v>
+        <v>0.5735812803590546</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5280812406997041</v>
+        <v>0.7573514906297172</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7266919847498692</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.3433641560179854</v>
+        <v>0.3358430848771266</v>
       </c>
     </row>
   </sheetData>
@@ -1430,7 +1390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1441,53 +1401,45 @@
     <row r="1">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>K óptimo knnpp</t>
+          <t>K óptimo</t>
         </is>
       </c>
       <c r="B1" s="3" t="inlineStr">
         <is>
-          <t>Arreglo aleatorio óptimo knnpp</t>
+          <t>MAE knnpp</t>
         </is>
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>MAE knnpp</t>
+          <t>MSE knnpp</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
         <is>
-          <t>MSE knnpp</t>
+          <t>RMSE knnpp</t>
         </is>
       </c>
       <c r="E1" s="3" t="inlineStr">
         <is>
-          <t>RMSE knnpp</t>
-        </is>
-      </c>
-      <c r="F1" s="3" t="inlineStr">
-        <is>
-          <t>R-cuadrado knnpp</t>
+          <t>R2 knnpp</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>73</v>
+        <v>0.7557783359119404</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7410072360200077</v>
+        <v>0.8315282410723833</v>
       </c>
       <c r="D2" t="n">
-        <v>1.109972397053677</v>
+        <v>0.9118817034420547</v>
       </c>
       <c r="E2" t="n">
-        <v>1.053552275425229</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.1469231795922281</v>
+        <v>0.03716308335154872</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
estoy arreglando la forma de eleccion de modelo del modelo de arbol a la forma en el evaluo los de regresion
</commit_message>
<xml_diff>
--- a/resultadospython.xlsx
+++ b/resultadospython.xlsx
@@ -989,16 +989,16 @@
         <v>122</v>
       </c>
       <c r="B2" t="n">
-        <v>0.4573004169495208</v>
+        <v>0.4583290788826664</v>
       </c>
       <c r="C2" t="n">
-        <v>0.410033964531995</v>
+        <v>0.410241144989027</v>
       </c>
       <c r="D2" t="n">
-        <v>0.6403389450377004</v>
+        <v>0.6405006986639648</v>
       </c>
       <c r="E2" t="n">
-        <v>0.6226367865212324</v>
+        <v>0.6224461138214116</v>
       </c>
     </row>
   </sheetData>
@@ -1115,16 +1115,16 @@
         <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>0.5774729620742622</v>
+        <v>0.5664313171976088</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6466338346268923</v>
+        <v>0.5982123173087937</v>
       </c>
       <c r="D2" t="n">
-        <v>0.8041354578843618</v>
+        <v>0.7734418642075135</v>
       </c>
       <c r="E2" t="n">
-        <v>0.3648838465338654</v>
+        <v>0.4124428918192228</v>
       </c>
     </row>
   </sheetData>
@@ -1178,16 +1178,16 @@
         <v>115</v>
       </c>
       <c r="B2" t="n">
-        <v>0.4293526781499747</v>
+        <v>0.4295092022072674</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3504596228933595</v>
+        <v>0.3504380316051455</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5919963031078483</v>
+        <v>0.5919780668277715</v>
       </c>
       <c r="E2" t="n">
-        <v>0.6557826768132963</v>
+        <v>0.6558038835228504</v>
       </c>
     </row>
   </sheetData>
@@ -1304,16 +1304,16 @@
         <v>6</v>
       </c>
       <c r="B2" t="n">
-        <v>0.775569221353989</v>
+        <v>0.7708994618676629</v>
       </c>
       <c r="C2" t="n">
-        <v>1.827375618630338</v>
+        <v>1.875120075338438</v>
       </c>
       <c r="D2" t="n">
-        <v>1.351804578565385</v>
+        <v>1.369350238375281</v>
       </c>
       <c r="E2" t="n">
-        <v>-1.115941009930692</v>
+        <v>-1.171224911562941</v>
       </c>
     </row>
   </sheetData>
@@ -1367,16 +1367,16 @@
         <v>110</v>
       </c>
       <c r="B2" t="n">
-        <v>0.6276056324687056</v>
+        <v>0.6279822259756672</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5735812803590546</v>
+        <v>0.5739241681786854</v>
       </c>
       <c r="D2" t="n">
-        <v>0.7573514906297172</v>
+        <v>0.7575778297829771</v>
       </c>
       <c r="E2" t="n">
-        <v>0.3358430848771266</v>
+        <v>0.3354460507961389</v>
       </c>
     </row>
   </sheetData>
@@ -2563,22 +2563,22 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B2" t="n">
-        <v>0.6060606060606061</v>
+        <v>0.6121212121212121</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5653433616742969</v>
+        <v>0.5668831168831169</v>
       </c>
       <c r="D2" t="n">
-        <v>0.6060606060606061</v>
+        <v>0.6121212121212121</v>
       </c>
       <c r="E2" t="n">
-        <v>0.542436518809878</v>
+        <v>0.5456423347490885</v>
       </c>
       <c r="F2" t="n">
-        <v>0.771043771043771</v>
+        <v>0.7710927456382002</v>
       </c>
     </row>
   </sheetData>
@@ -2727,16 +2727,16 @@
         <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>0.8708212942316997</v>
+        <v>0.8885700370022505</v>
       </c>
       <c r="C2" t="n">
-        <v>1.385562392002157</v>
+        <v>1.40324588947056</v>
       </c>
       <c r="D2" t="n">
-        <v>1.177099142809201</v>
+        <v>1.184586801154968</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.6717157196487737</v>
+        <v>-0.6930513021291713</v>
       </c>
     </row>
   </sheetData>
@@ -2787,19 +2787,19 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B2" t="n">
-        <v>0.6290313206092344</v>
+        <v>0.6327999337790693</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6401813750093149</v>
+        <v>0.6461734745561803</v>
       </c>
       <c r="D2" t="n">
-        <v>0.8001133513504914</v>
+        <v>0.8038491615696196</v>
       </c>
       <c r="E2" t="n">
-        <v>0.2276051412719259</v>
+        <v>0.2203755231298511</v>
       </c>
     </row>
   </sheetData>
@@ -2853,16 +2853,16 @@
         <v>23</v>
       </c>
       <c r="B2" t="n">
-        <v>0.6465181857472143</v>
+        <v>0.6465181857472145</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7076411505920056</v>
+        <v>0.7076411505920059</v>
       </c>
       <c r="D2" t="n">
-        <v>0.8412140931962597</v>
+        <v>0.8412140931962599</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1462132328768061</v>
+        <v>0.1462132328768058</v>
       </c>
     </row>
   </sheetData>
@@ -2913,19 +2913,19 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>0.6845854597204523</v>
+        <v>0.6798361056886949</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7617854841998375</v>
+        <v>0.7604864217832062</v>
       </c>
       <c r="D2" t="n">
-        <v>0.8728032333807189</v>
+        <v>0.8720587261092032</v>
       </c>
       <c r="E2" t="n">
-        <v>0.2989121800501523</v>
+        <v>0.3001077355661667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
estoy corrigiendo la tabla de resultados de python va primero RMSE, MAE, R2 y MSE
</commit_message>
<xml_diff>
--- a/resultadospython.xlsx
+++ b/resultadospython.xlsx
@@ -8,28 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a57f4c5e645b2417/1 A NMI/3 InvestigacionMia/F Métodos predictivos con ML/A Codigo/Comparacion_de_metodos_predictivos/crispy-invention_metodos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_A2930E9B52BD7D22DF06529C783CFC6B5C9FDC5E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59ADC428-0A7E-CA49-A54E-2D666B3C03CC}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="11_A2930E9B52BD7D22DF06529C783CFC6B5C9FDC5E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1D80EBB-527B-0544-8A77-D27FD7A04604}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="895" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15720" tabRatio="895" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ResltCategoricas" sheetId="1" r:id="rId1"/>
     <sheet name="ResltNumericas" sheetId="2" r:id="rId2"/>
-    <sheet name="arbolu" sheetId="3" r:id="rId3"/>
-    <sheet name="bosqueu" sheetId="4" r:id="rId4"/>
-    <sheet name="knnu" sheetId="5" r:id="rId5"/>
-    <sheet name="arbolts" sheetId="6" r:id="rId6"/>
-    <sheet name="bosquets" sheetId="7" r:id="rId7"/>
-    <sheet name="knnts" sheetId="8" r:id="rId8"/>
-    <sheet name="arboltd" sheetId="9" r:id="rId9"/>
-    <sheet name="bosquetd" sheetId="10" r:id="rId10"/>
-    <sheet name="knntd" sheetId="11" r:id="rId11"/>
-    <sheet name="arbolcc" sheetId="12" r:id="rId12"/>
-    <sheet name="bosquecc" sheetId="13" r:id="rId13"/>
-    <sheet name="knncc" sheetId="14" r:id="rId14"/>
-    <sheet name="arbolpp" sheetId="15" r:id="rId15"/>
-    <sheet name="bosquepp" sheetId="16" r:id="rId16"/>
-    <sheet name="knnpp" sheetId="17" r:id="rId17"/>
+    <sheet name="Resultados" sheetId="18" r:id="rId3"/>
+    <sheet name="arbolu" sheetId="3" r:id="rId4"/>
+    <sheet name="bosqueu" sheetId="4" r:id="rId5"/>
+    <sheet name="knnu" sheetId="5" r:id="rId6"/>
+    <sheet name="arbolts" sheetId="6" r:id="rId7"/>
+    <sheet name="bosquets" sheetId="7" r:id="rId8"/>
+    <sheet name="knnts" sheetId="8" r:id="rId9"/>
+    <sheet name="arboltd" sheetId="9" r:id="rId10"/>
+    <sheet name="bosquetd" sheetId="10" r:id="rId11"/>
+    <sheet name="knntd" sheetId="11" r:id="rId12"/>
+    <sheet name="arbolcc" sheetId="12" r:id="rId13"/>
+    <sheet name="bosquecc" sheetId="13" r:id="rId14"/>
+    <sheet name="knncc" sheetId="14" r:id="rId15"/>
+    <sheet name="arbolpp" sheetId="15" r:id="rId16"/>
+    <sheet name="bosquepp" sheetId="16" r:id="rId17"/>
+    <sheet name="knnpp" sheetId="17" r:id="rId18"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="105">
   <si>
     <t>..</t>
   </si>
@@ -462,7 +463,94 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="47">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
@@ -587,11 +675,46 @@
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Arreglo aleatorio óptimo"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Exactitud media"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Desviación estándar de la exactitud"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Exactitud" dataDxfId="25"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Precisión" dataDxfId="24"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Sensibilidad" dataDxfId="23"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="F1-score" dataDxfId="22"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="ROC/AUC" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Exactitud" dataDxfId="46"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Precisión" dataDxfId="45"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Sensibilidad" dataDxfId="44"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="F1-score" dataDxfId="43"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="ROC/AUC" dataDxfId="42"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium8" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{F4803572-78D3-5E4A-8CDF-7E1839A9B76A}" name="Tabla1711" displayName="Tabla1711" ref="B22:H25" totalsRowShown="0">
+  <autoFilter ref="B22:H25" xr:uid="{F4803572-78D3-5E4A-8CDF-7E1839A9B76A}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{B9E3B94D-F2EF-B84C-8882-10E6B0FE8800}" name="perimetro de pantorrilla"/>
+    <tableColumn id="2" xr3:uid="{9EE19DA1-001C-AA40-8722-DF5BFA1888D3}" name="Profundidad óptima"/>
+    <tableColumn id="3" xr3:uid="{A607CD5A-244A-6A4E-8755-AE120E7A408C}" name="Arreglo aleatorio óptimo"/>
+    <tableColumn id="4" xr3:uid="{7C2E0ADD-06EB-C74F-9158-CA6E5324988D}" name="RMSE" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{586688CE-46E1-4144-9FEA-BAB90597A5FE}" name="MAE" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{492A1A93-289E-C240-84E8-5E31D6117DE6}" name="R2" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{E5D6433C-B6A3-CD45-8C37-A21936E3B61D}" name="MSE" dataDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{AE2DDEAD-8ACD-B54D-AABA-0419B034BB17}" name="Tabla13712" displayName="Tabla13712" ref="B2:K5" totalsRowShown="0">
+  <autoFilter ref="B2:K5" xr:uid="{AE2DDEAD-8ACD-B54D-AABA-0419B034BB17}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{8591D46B-E210-9742-AF73-191D28190F45}" name="turno"/>
+    <tableColumn id="2" xr3:uid="{FF1BB84F-3D4C-2B44-822E-C0068EB05C43}" name="Hiperparametro"/>
+    <tableColumn id="3" xr3:uid="{EEE4CD31-2FFC-354E-8B04-C5FB8AFEC644}" name="Arreglo aleatorio óptimo"/>
+    <tableColumn id="4" xr3:uid="{3DCC5FAF-7469-2049-8A53-45CB5090D537}" name="Exactitud media"/>
+    <tableColumn id="5" xr3:uid="{254891EC-97CC-CB43-A9CB-789B93BCA29A}" name="Desviación estándar de la exactitud"/>
+    <tableColumn id="6" xr3:uid="{13FABB82-1426-1B47-BEE2-3E3137860AD1}" name="Exactitud" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{92346E6C-FF9E-8F44-8E88-0D2D11FA6629}" name="Precisión" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{3FB12E74-5615-8C41-9CBD-659CA9277DBF}" name="Sensibilidad" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{5D813947-52FE-1949-A52F-BAD21E821771}" name="F1-score" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{94D4E7BE-6F35-5A47-9FCC-7509FFCC2F8A}" name="ROC/AUC" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -604,10 +727,10 @@
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="tension sistolia"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Profundidad óptima"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Arreglo aleatorio óptimo"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="RMSE" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="MAE" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="R2" dataDxfId="18"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="MSE" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="RMSE" dataDxfId="41"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="MAE" dataDxfId="40"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="R2" dataDxfId="39"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="MSE" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -620,10 +743,10 @@
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="tension diastolica"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Profundidad óptima"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Arreglo aleatorio óptimo"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="RMSE" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="MAE" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="R2" dataDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="MSE" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="RMSE" dataDxfId="37"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="MAE" dataDxfId="36"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="R2" dataDxfId="35"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="MSE" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -636,10 +759,10 @@
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="circunferencia de cintura"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Profundidad óptima"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Arreglo aleatorio óptimo"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="RMSE" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="MAE" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="R2" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="MSE" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="RMSE" dataDxfId="33"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="MAE" dataDxfId="32"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="R2" dataDxfId="31"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="MSE" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -652,10 +775,10 @@
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="perimetro de pantorrilla"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Profundidad óptima"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Arreglo aleatorio óptimo"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="RMSE" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="MAE" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="R2" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="MSE" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="RMSE" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="MAE" dataDxfId="28"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="R2" dataDxfId="27"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="MSE" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -670,13 +793,61 @@
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Arreglo aleatorio óptimo"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Exactitud media"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Desviación estándar de la exactitud"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Exactitud" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Precisión" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="Sensibilidad" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0500-000009000000}" name="F1-score" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0500-00000A000000}" name="ROC/AUC" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Exactitud" dataDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Precisión" dataDxfId="24"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="Sensibilidad" dataDxfId="23"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0500-000009000000}" name="F1-score" dataDxfId="22"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0500-00000A000000}" name="ROC/AUC" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{1C1EC2A6-3C72-044E-85E2-66ED6143EB65}" name="Tabla148" displayName="Tabla148" ref="B7:H10" totalsRowShown="0">
+  <autoFilter ref="B7:H10" xr:uid="{1C1EC2A6-3C72-044E-85E2-66ED6143EB65}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{2EC7241C-E812-8441-BDAE-63FD69409946}" name="tension sistolia"/>
+    <tableColumn id="2" xr3:uid="{27042E5E-8951-9647-93EF-CA198F29C7BA}" name="Profundidad óptima"/>
+    <tableColumn id="3" xr3:uid="{D11FB627-5040-7346-9FF9-D4DF52A319CE}" name="Arreglo aleatorio óptimo"/>
+    <tableColumn id="4" xr3:uid="{CB05180F-D529-2541-BA8C-9042950AAB54}" name="RMSE" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{6669C8B9-BA57-E94C-83B2-2EBC43DBAF89}" name="MAE" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{6A7315A2-0322-3C4D-8441-43F5FAE71F58}" name="R2" dataDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{B71E0582-FB14-0140-B5A0-251C74324786}" name="MSE" dataDxfId="17"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{5BFA5D43-4A63-8F44-A86F-95ECD9B82AB6}" name="Tabla159" displayName="Tabla159" ref="B12:H15" totalsRowShown="0">
+  <autoFilter ref="B12:H15" xr:uid="{5BFA5D43-4A63-8F44-A86F-95ECD9B82AB6}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{E65838A9-E947-E342-A29D-6D06E84732AA}" name="tension diastolica"/>
+    <tableColumn id="2" xr3:uid="{C0808544-A92A-F444-8E3B-B20829B88C51}" name="Profundidad óptima"/>
+    <tableColumn id="3" xr3:uid="{AE7927B5-5B06-6C48-B332-3A11B18D54FE}" name="Arreglo aleatorio óptimo"/>
+    <tableColumn id="4" xr3:uid="{51CD5BCB-38C8-C34B-A09E-5E7C3E68C730}" name="RMSE" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{CD7C7117-16A9-BB4B-824A-245F8409B991}" name="MAE" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{F5767FE9-D290-DA4D-BF62-9A8C994F2479}" name="R2" dataDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{65AA60C5-51FD-B543-BEE1-DC2D1DB3D1FC}" name="MSE" dataDxfId="13"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{D01FE413-F807-6842-B5DD-1A4270E262AA}" name="Tabla1610" displayName="Tabla1610" ref="B17:H20" totalsRowShown="0">
+  <autoFilter ref="B17:H20" xr:uid="{D01FE413-F807-6842-B5DD-1A4270E262AA}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{E5FD783A-EAE2-3444-B09F-EBF8E923F927}" name="circunferencia de cintura"/>
+    <tableColumn id="2" xr3:uid="{BC30B3EA-B103-C646-88B1-F5CFBEA729D3}" name="Profundidad óptima"/>
+    <tableColumn id="3" xr3:uid="{5F11433F-E58D-004B-A75E-1FDE85AD1CF1}" name="Arreglo aleatorio óptimo"/>
+    <tableColumn id="4" xr3:uid="{DA18C714-96F5-0D4A-8CE5-2CA2D520F955}" name="RMSE" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{E6AD2BD8-577B-3F4E-ADBF-0FDB872ABD97}" name="MAE" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{B14CC969-6517-CE4E-A8EA-447AD21A5E87}" name="R2" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{196E1079-27CE-4A43-92A9-B4DA6DA04726}" name="MSE" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -966,12 +1137,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
-    <tabColor rgb="FF00B050"/>
+    <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1213,7 +1384,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1222,36 +1393,36 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>122</v>
+        <v>3</v>
       </c>
       <c r="B2">
-        <v>0.45832907888266639</v>
+        <v>0.6798361056886949</v>
       </c>
       <c r="C2">
-        <v>0.41024114498902697</v>
+        <v>0.76048642178320625</v>
       </c>
       <c r="D2">
-        <v>0.64050069866396475</v>
+        <v>0.87205872610920321</v>
       </c>
       <c r="E2">
-        <v>0.62244611382141157</v>
+        <v>0.30010773556616671</v>
       </c>
     </row>
   </sheetData>
@@ -1260,6 +1431,55 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>122</v>
+      </c>
+      <c r="B2">
+        <v>0.45832907888266639</v>
+      </c>
+      <c r="C2">
+        <v>0.41024114498902697</v>
+      </c>
+      <c r="D2">
+        <v>0.64050069866396475</v>
+      </c>
+      <c r="E2">
+        <v>0.62244611382141157</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1306,7 +1526,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1353,7 +1573,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1400,7 +1620,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1447,7 +1667,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1494,7 +1714,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1541,7 +1761,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1591,12 +1811,12 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
-    <tabColor rgb="FFFF0000"/>
+    <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:P36"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="158" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection sqref="A1:K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2692,12 +2912,912 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DE89837-C912-794F-A747-38AF6996C5DA}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:K25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" customWidth="1"/>
+    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <f>arbolu!A2</f>
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <f>arbolu!B2</f>
+        <v>0.61212121212121207</v>
+      </c>
+      <c r="E3">
+        <f>arbolu!C2</f>
+        <v>0.41197063805759448</v>
+      </c>
+      <c r="F3">
+        <f>arbolu!D2</f>
+        <v>0.61212121212121207</v>
+      </c>
+      <c r="G3" s="1">
+        <f>arbolu!E2</f>
+        <v>0.48260789715335167</v>
+      </c>
+      <c r="H3" s="1">
+        <f>arbolu!F2</f>
+        <v>0.77411692684419953</v>
+      </c>
+      <c r="I3" s="1">
+        <f>arbolu!G2</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <f>arbolu!H2</f>
+        <v>0</v>
+      </c>
+      <c r="K3" s="1">
+        <f>arbolu!I2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <f>bosqueu!A2</f>
+        <v>108</v>
+      </c>
+      <c r="D4">
+        <f>bosqueu!B2</f>
+        <v>0.61212121212121207</v>
+      </c>
+      <c r="E4">
+        <f>bosqueu!C2</f>
+        <v>0.56688311688311688</v>
+      </c>
+      <c r="F4">
+        <f>bosqueu!D2</f>
+        <v>0.61212121212121207</v>
+      </c>
+      <c r="G4" s="1">
+        <f>bosqueu!E2</f>
+        <v>0.54564233474908852</v>
+      </c>
+      <c r="H4" s="1">
+        <f>bosqueu!F2</f>
+        <v>0.77109274563820018</v>
+      </c>
+      <c r="I4" s="1">
+        <f>bosqueu!G2</f>
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <f>bosqueu!H2</f>
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <f>bosqueu!I2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <f>knnu!A2</f>
+        <v>23</v>
+      </c>
+      <c r="D5">
+        <f>knnu!B2</f>
+        <v>38</v>
+      </c>
+      <c r="E5">
+        <f>knnu!C2</f>
+        <v>0.55882352941176472</v>
+      </c>
+      <c r="F5">
+        <f>knnu!D2</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <f>knnu!E2</f>
+        <v>0.55882352941176472</v>
+      </c>
+      <c r="H5" s="1">
+        <f>knnu!F2</f>
+        <v>0.31228373702422152</v>
+      </c>
+      <c r="I5" s="1">
+        <f>knnu!G2</f>
+        <v>0.55882352941176472</v>
+      </c>
+      <c r="J5" s="1">
+        <f>knnu!H2</f>
+        <v>0.40066592674805768</v>
+      </c>
+      <c r="K5" s="1">
+        <f>knnu!I2</f>
+        <v>0.81660899653979235</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8">
+        <f>arbolts!A2</f>
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <f>arbolts!B2</f>
+        <v>0.88857003700225046</v>
+      </c>
+      <c r="E8" s="1">
+        <f>arbolts!E2</f>
+        <v>-0.69305130212917132</v>
+      </c>
+      <c r="F8" s="1">
+        <f>arbolts!C2</f>
+        <v>1.4032458894705599</v>
+      </c>
+      <c r="G8" s="1">
+        <f>arbolts!F2</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <f>arbolts!D2</f>
+        <v>1.1845868011549681</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9">
+        <f>bosquets!A2</f>
+        <v>123</v>
+      </c>
+      <c r="D9">
+        <f>bosquets!B2</f>
+        <v>0.63279993377906929</v>
+      </c>
+      <c r="E9" s="1">
+        <f>bosquets!E2</f>
+        <v>0.22037552312985109</v>
+      </c>
+      <c r="F9" s="1">
+        <f>bosquets!C2</f>
+        <v>0.64617347455618035</v>
+      </c>
+      <c r="G9" s="1">
+        <f>bosquets!F2</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <f>bosquets!D2</f>
+        <v>0.80384916156961961</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10">
+        <f>knnts!A2</f>
+        <v>23</v>
+      </c>
+      <c r="D10">
+        <f>knnts!B2</f>
+        <v>0.64651818574721454</v>
+      </c>
+      <c r="E10" s="1">
+        <f>knnts!E2</f>
+        <v>0.14621323287680579</v>
+      </c>
+      <c r="F10" s="1">
+        <f>knnts!C2</f>
+        <v>0.70764115059200594</v>
+      </c>
+      <c r="G10" s="1">
+        <f>knnts!F2</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <f>knnts!D2</f>
+        <v>0.84121409319625995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13">
+        <f>arboltd!A2</f>
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <f>arboltd!B2</f>
+        <v>0.6798361056886949</v>
+      </c>
+      <c r="E13" s="1">
+        <f>arboltd!E2</f>
+        <v>0.30010773556616671</v>
+      </c>
+      <c r="F13" s="1">
+        <f>arboltd!C2</f>
+        <v>0.76048642178320625</v>
+      </c>
+      <c r="G13" s="1">
+        <f>arboltd!F2</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="1">
+        <f>arboltd!D2</f>
+        <v>0.87205872610920321</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14">
+        <f>bosquetd!A2</f>
+        <v>122</v>
+      </c>
+      <c r="D14">
+        <f>bosquetd!B2</f>
+        <v>0.45832907888266639</v>
+      </c>
+      <c r="E14" s="1">
+        <f>bosquetd!E2</f>
+        <v>0.62244611382141157</v>
+      </c>
+      <c r="F14" s="1">
+        <f>bosquetd!C2</f>
+        <v>0.41024114498902697</v>
+      </c>
+      <c r="G14" s="1">
+        <f>bosquetd!F2</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <f>bosquetd!D2</f>
+        <v>0.64050069866396475</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15">
+        <f>knntd!A2</f>
+        <v>15</v>
+      </c>
+      <c r="D15">
+        <f>knntd!B2</f>
+        <v>0.62201029721223688</v>
+      </c>
+      <c r="E15" s="1">
+        <f>knntd!E2</f>
+        <v>0.37251040538711189</v>
+      </c>
+      <c r="F15" s="1">
+        <f>knntd!C2</f>
+        <v>0.68181538897185989</v>
+      </c>
+      <c r="G15" s="1">
+        <f>knntd!F2</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
+        <f>knntd!D2</f>
+        <v>0.82572113269060754</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18">
+        <f>arbolcc!A2</f>
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <f>arbolcc!B2</f>
+        <v>0.56643131719760875</v>
+      </c>
+      <c r="E18" s="1">
+        <f>arbolcc!E2</f>
+        <v>0.41244289181922278</v>
+      </c>
+      <c r="F18" s="1">
+        <f>arbolcc!C2</f>
+        <v>0.59821231730879365</v>
+      </c>
+      <c r="G18" s="1">
+        <f>arbolcc!F2</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="1">
+        <f>arbolcc!D2</f>
+        <v>0.77344186420751349</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19">
+        <f>bosquecc!A2</f>
+        <v>115</v>
+      </c>
+      <c r="D19">
+        <f>bosquecc!B2</f>
+        <v>0.4295092022072674</v>
+      </c>
+      <c r="E19" s="1">
+        <f>bosquecc!E2</f>
+        <v>0.65580388352285035</v>
+      </c>
+      <c r="F19" s="1">
+        <f>bosquecc!C2</f>
+        <v>0.35043803160514547</v>
+      </c>
+      <c r="G19" s="1">
+        <f>bosquecc!F2</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="1">
+        <f>bosquecc!D2</f>
+        <v>0.59197806682777154</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20">
+        <f>knncc!A2</f>
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <f>knncc!B2</f>
+        <v>0.53264070017665743</v>
+      </c>
+      <c r="E20" s="1">
+        <f>knncc!E2</f>
+        <v>0.5284551380655178</v>
+      </c>
+      <c r="F20" s="1">
+        <f>knncc!C2</f>
+        <v>0.48009621642785288</v>
+      </c>
+      <c r="G20" s="1">
+        <f>knncc!F2</f>
+        <v>0</v>
+      </c>
+      <c r="H20" s="1">
+        <f>knncc!D2</f>
+        <v>0.69288975777381279</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G22" t="s">
+        <v>19</v>
+      </c>
+      <c r="H22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23">
+        <f>arbolpp!A2</f>
+        <v>6</v>
+      </c>
+      <c r="D23">
+        <f>arbolpp!B2</f>
+        <v>0.77089946186766289</v>
+      </c>
+      <c r="E23" s="1">
+        <f>arbolpp!E2</f>
+        <v>-1.171224911562941</v>
+      </c>
+      <c r="F23" s="1">
+        <f>arbolpp!C2</f>
+        <v>1.8751200753384381</v>
+      </c>
+      <c r="G23" s="1">
+        <f>arbolpp!F2</f>
+        <v>0</v>
+      </c>
+      <c r="H23" s="1">
+        <f>arbolpp!D2</f>
+        <v>1.3693502383752809</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24">
+        <f>bosquepp!A2</f>
+        <v>110</v>
+      </c>
+      <c r="D24">
+        <f>bosquepp!B2</f>
+        <v>0.62798222597566722</v>
+      </c>
+      <c r="E24" s="1">
+        <f>bosquepp!E2</f>
+        <v>0.33544605079613887</v>
+      </c>
+      <c r="F24" s="1">
+        <f>bosquepp!C2</f>
+        <v>0.57392416817868541</v>
+      </c>
+      <c r="G24" s="1">
+        <f>bosquepp!F2</f>
+        <v>0</v>
+      </c>
+      <c r="H24" s="1">
+        <f>bosquepp!D2</f>
+        <v>0.75757782978297705</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25">
+        <f>knnpp!A2</f>
+        <v>5</v>
+      </c>
+      <c r="D25">
+        <f>knnpp!B2</f>
+        <v>0.75577833591194044</v>
+      </c>
+      <c r="E25" s="1">
+        <f>knnpp!E2</f>
+        <v>3.716308335154872E-2</v>
+      </c>
+      <c r="F25" s="1">
+        <f>knnpp!C2</f>
+        <v>0.83152824107238332</v>
+      </c>
+      <c r="G25" s="1">
+        <f>knnpp!F2</f>
+        <v>0</v>
+      </c>
+      <c r="H25" s="1">
+        <f>knnpp!D2</f>
+        <v>0.91188170344205466</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E8:E10">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13:E15">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E18:E20">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E23:E25">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8:F10">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F13:F15">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F18:F20">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F23:F25">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G5">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G8:G10">
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G13:G15">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G18:G20">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G23:G25">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:H5">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H8:H10">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H13:H15">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H18:H20">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H23:H25">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3:I5">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:J5">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3:K5">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="5">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
@@ -2744,11 +3864,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -2797,7 +3919,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
@@ -2868,11 +3990,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -2915,13 +4039,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="270" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
@@ -2962,7 +4094,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -3007,51 +4139,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>3</v>
-      </c>
-      <c r="B2">
-        <v>0.6798361056886949</v>
-      </c>
-      <c r="C2">
-        <v>0.76048642178320625</v>
-      </c>
-      <c r="D2">
-        <v>0.87205872610920321</v>
-      </c>
-      <c r="E2">
-        <v>0.30010773556616671</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
corregir la tabla resultadospython para esa tabla ponerla en el word y continuar con la parte de tablas, graficas y figuras
</commit_message>
<xml_diff>
--- a/resultadospython.xlsx
+++ b/resultadospython.xlsx
@@ -1,36 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a57f4c5e645b2417/1 A NMI/3 InvestigacionMia/F Métodos predictivos con ML/A Codigo/Comparacion_de_metodos_predictivos/crispy-invention_metodos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a57f4c5e645b2417/1 A NMI/3 InvestigacionMia/F Métodos predictivos con ML/A Codigo/Comparacion_de_metodos_predictivos/crispy-invention_metodos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="11_A2930E9B52BD7D22DF06529C783CFC6B5C9FDC5E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1D80EBB-527B-0544-8A77-D27FD7A04604}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="11_56D39CBB14DFCB49F4F7AA771C19E857CCB753F9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60E0061B-783A-4676-BF89-267FFAC41AF1}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15720" tabRatio="895" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="895" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ResltCategoricas" sheetId="1" r:id="rId1"/>
     <sheet name="ResltNumericas" sheetId="2" r:id="rId2"/>
-    <sheet name="Resultados" sheetId="18" r:id="rId3"/>
-    <sheet name="arbolu" sheetId="3" r:id="rId4"/>
-    <sheet name="bosqueu" sheetId="4" r:id="rId5"/>
-    <sheet name="knnu" sheetId="5" r:id="rId6"/>
-    <sheet name="arbolts" sheetId="6" r:id="rId7"/>
-    <sheet name="bosquets" sheetId="7" r:id="rId8"/>
-    <sheet name="knnts" sheetId="8" r:id="rId9"/>
-    <sheet name="arboltd" sheetId="9" r:id="rId10"/>
-    <sheet name="bosquetd" sheetId="10" r:id="rId11"/>
-    <sheet name="knntd" sheetId="11" r:id="rId12"/>
-    <sheet name="arbolcc" sheetId="12" r:id="rId13"/>
-    <sheet name="bosquecc" sheetId="13" r:id="rId14"/>
-    <sheet name="knncc" sheetId="14" r:id="rId15"/>
-    <sheet name="arbolpp" sheetId="15" r:id="rId16"/>
-    <sheet name="bosquepp" sheetId="16" r:id="rId17"/>
-    <sheet name="knnpp" sheetId="17" r:id="rId18"/>
+    <sheet name="Resultados" sheetId="3" r:id="rId3"/>
+    <sheet name="arbolu" sheetId="4" r:id="rId4"/>
+    <sheet name="bosqueu" sheetId="5" r:id="rId5"/>
+    <sheet name="knnu" sheetId="6" r:id="rId6"/>
+    <sheet name="arbolts" sheetId="7" r:id="rId7"/>
+    <sheet name="bosquets" sheetId="8" r:id="rId8"/>
+    <sheet name="knnts" sheetId="9" r:id="rId9"/>
+    <sheet name="arboltd" sheetId="10" r:id="rId10"/>
+    <sheet name="bosquetd" sheetId="11" r:id="rId11"/>
+    <sheet name="knntd" sheetId="12" r:id="rId12"/>
+    <sheet name="arbolcc" sheetId="13" r:id="rId13"/>
+    <sheet name="bosquecc" sheetId="14" r:id="rId14"/>
+    <sheet name="knncc" sheetId="15" r:id="rId15"/>
+    <sheet name="arbolpp" sheetId="16" r:id="rId16"/>
+    <sheet name="bosquepp" sheetId="17" r:id="rId17"/>
+    <sheet name="knnpp" sheetId="18" r:id="rId18"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="105">
   <si>
     <t>..</t>
   </si>
@@ -232,16 +232,16 @@
     <t>R2 arbolts</t>
   </si>
   <si>
+    <t>RMSE bosquets</t>
+  </si>
+  <si>
     <t>MAE bosquets</t>
   </si>
   <si>
+    <t>R2 bosquets</t>
+  </si>
+  <si>
     <t>MSE bosquets</t>
-  </si>
-  <si>
-    <t>RMSE bosquets</t>
-  </si>
-  <si>
-    <t>R2 bosquets</t>
   </si>
   <si>
     <t>K óptimo</t>
@@ -465,6 +465,9 @@
   </cellStyles>
   <dxfs count="47">
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
@@ -532,9 +535,6 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -686,35 +686,32 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{F4803572-78D3-5E4A-8CDF-7E1839A9B76A}" name="Tabla1711" displayName="Tabla1711" ref="B22:H25" totalsRowShown="0">
-  <autoFilter ref="B22:H25" xr:uid="{F4803572-78D3-5E4A-8CDF-7E1839A9B76A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Tabla1711" displayName="Tabla1711" ref="B22:H25" totalsRowShown="0">
+  <autoFilter ref="B22:H25" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{B9E3B94D-F2EF-B84C-8882-10E6B0FE8800}" name="perimetro de pantorrilla"/>
-    <tableColumn id="2" xr3:uid="{9EE19DA1-001C-AA40-8722-DF5BFA1888D3}" name="Profundidad óptima"/>
-    <tableColumn id="3" xr3:uid="{A607CD5A-244A-6A4E-8755-AE120E7A408C}" name="Arreglo aleatorio óptimo"/>
-    <tableColumn id="4" xr3:uid="{7C2E0ADD-06EB-C74F-9158-CA6E5324988D}" name="RMSE" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{586688CE-46E1-4144-9FEA-BAB90597A5FE}" name="MAE" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{492A1A93-289E-C240-84E8-5E31D6117DE6}" name="R2" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{E5D6433C-B6A3-CD45-8C37-A21936E3B61D}" name="MSE" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="perimetro de pantorrilla"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="Profundidad óptima"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="Arreglo aleatorio óptimo"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="RMSE" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0900-000005000000}" name="MAE" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0900-000006000000}" name="R2" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0900-000007000000}" name="MSE" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{AE2DDEAD-8ACD-B54D-AABA-0419B034BB17}" name="Tabla13712" displayName="Tabla13712" ref="B2:K5" totalsRowShown="0">
-  <autoFilter ref="B2:K5" xr:uid="{AE2DDEAD-8ACD-B54D-AABA-0419B034BB17}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{8591D46B-E210-9742-AF73-191D28190F45}" name="turno"/>
-    <tableColumn id="2" xr3:uid="{FF1BB84F-3D4C-2B44-822E-C0068EB05C43}" name="Hiperparametro"/>
-    <tableColumn id="3" xr3:uid="{EEE4CD31-2FFC-354E-8B04-C5FB8AFEC644}" name="Arreglo aleatorio óptimo"/>
-    <tableColumn id="4" xr3:uid="{3DCC5FAF-7469-2049-8A53-45CB5090D537}" name="Exactitud media"/>
-    <tableColumn id="5" xr3:uid="{254891EC-97CC-CB43-A9CB-789B93BCA29A}" name="Desviación estándar de la exactitud"/>
-    <tableColumn id="6" xr3:uid="{13FABB82-1426-1B47-BEE2-3E3137860AD1}" name="Exactitud" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{92346E6C-FF9E-8F44-8E88-0D2D11FA6629}" name="Precisión" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{3FB12E74-5615-8C41-9CBD-659CA9277DBF}" name="Sensibilidad" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{5D813947-52FE-1949-A52F-BAD21E821771}" name="F1-score" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{94D4E7BE-6F35-5A47-9FCC-7509FFCC2F8A}" name="ROC/AUC" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="Tabla13712" displayName="Tabla13712" ref="B2:H5" totalsRowShown="0">
+  <autoFilter ref="B2:H5" xr:uid="{00000000-0009-0000-0100-00000B000000}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="turno"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="Hiperparametro"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0A00-000006000000}" name="Exactitud" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0A00-000007000000}" name="Precisión" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0A00-000008000000}" name="Sensibilidad" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0A00-000009000000}" name="F1-score" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0A00-00000A000000}" name="ROC/AUC" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -804,48 +801,48 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{1C1EC2A6-3C72-044E-85E2-66ED6143EB65}" name="Tabla148" displayName="Tabla148" ref="B7:H10" totalsRowShown="0">
-  <autoFilter ref="B7:H10" xr:uid="{1C1EC2A6-3C72-044E-85E2-66ED6143EB65}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Tabla148" displayName="Tabla148" ref="B7:H10" totalsRowShown="0">
+  <autoFilter ref="B7:H10" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{2EC7241C-E812-8441-BDAE-63FD69409946}" name="tension sistolia"/>
-    <tableColumn id="2" xr3:uid="{27042E5E-8951-9647-93EF-CA198F29C7BA}" name="Profundidad óptima"/>
-    <tableColumn id="3" xr3:uid="{D11FB627-5040-7346-9FF9-D4DF52A319CE}" name="Arreglo aleatorio óptimo"/>
-    <tableColumn id="4" xr3:uid="{CB05180F-D529-2541-BA8C-9042950AAB54}" name="RMSE" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{6669C8B9-BA57-E94C-83B2-2EBC43DBAF89}" name="MAE" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{6A7315A2-0322-3C4D-8441-43F5FAE71F58}" name="R2" dataDxfId="18"/>
-    <tableColumn id="7" xr3:uid="{B71E0582-FB14-0140-B5A0-251C74324786}" name="MSE" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="tension sistolia"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Profundidad óptima"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="Arreglo aleatorio óptimo"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="RMSE" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="MAE" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="R2" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="MSE" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{5BFA5D43-4A63-8F44-A86F-95ECD9B82AB6}" name="Tabla159" displayName="Tabla159" ref="B12:H15" totalsRowShown="0">
-  <autoFilter ref="B12:H15" xr:uid="{5BFA5D43-4A63-8F44-A86F-95ECD9B82AB6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Tabla159" displayName="Tabla159" ref="B12:H15" totalsRowShown="0">
+  <autoFilter ref="B12:H15" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{E65838A9-E947-E342-A29D-6D06E84732AA}" name="tension diastolica"/>
-    <tableColumn id="2" xr3:uid="{C0808544-A92A-F444-8E3B-B20829B88C51}" name="Profundidad óptima"/>
-    <tableColumn id="3" xr3:uid="{AE7927B5-5B06-6C48-B332-3A11B18D54FE}" name="Arreglo aleatorio óptimo"/>
-    <tableColumn id="4" xr3:uid="{51CD5BCB-38C8-C34B-A09E-5E7C3E68C730}" name="RMSE" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{CD7C7117-16A9-BB4B-824A-245F8409B991}" name="MAE" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{F5767FE9-D290-DA4D-BF62-9A8C994F2479}" name="R2" dataDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{65AA60C5-51FD-B543-BEE1-DC2D1DB3D1FC}" name="MSE" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="tension diastolica"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Profundidad óptima"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Arreglo aleatorio óptimo"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="RMSE" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="MAE" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="R2" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="MSE" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{D01FE413-F807-6842-B5DD-1A4270E262AA}" name="Tabla1610" displayName="Tabla1610" ref="B17:H20" totalsRowShown="0">
-  <autoFilter ref="B17:H20" xr:uid="{D01FE413-F807-6842-B5DD-1A4270E262AA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Tabla1610" displayName="Tabla1610" ref="B17:H20" totalsRowShown="0">
+  <autoFilter ref="B17:H20" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{E5FD783A-EAE2-3444-B09F-EBF8E923F927}" name="circunferencia de cintura"/>
-    <tableColumn id="2" xr3:uid="{BC30B3EA-B103-C646-88B1-F5CFBEA729D3}" name="Profundidad óptima"/>
-    <tableColumn id="3" xr3:uid="{5F11433F-E58D-004B-A75E-1FDE85AD1CF1}" name="Arreglo aleatorio óptimo"/>
-    <tableColumn id="4" xr3:uid="{DA18C714-96F5-0D4A-8CE5-2CA2D520F955}" name="RMSE" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{E6AD2BD8-577B-3F4E-ADBF-0FDB872ABD97}" name="MAE" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{B14CC969-6517-CE4E-A8EA-447AD21A5E87}" name="R2" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{196E1079-27CE-4A43-92A9-B4DA6DA04726}" name="MSE" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="circunferencia de cintura"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="Profundidad óptima"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="Arreglo aleatorio óptimo"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="RMSE" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="MAE" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="R2" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0800-000007000000}" name="MSE" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1145,22 +1142,22 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="1" max="1" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" customWidth="1"/>
-    <col min="6" max="6" width="34.33203125" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="6" max="6" width="34.28515625" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -1192,7 +1189,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>11</v>
       </c>
@@ -1233,33 +1230,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>12</v>
       </c>
       <c r="C4">
         <f>bosqueu!A2</f>
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D4">
         <f>bosqueu!B2</f>
-        <v>0.61212121212121207</v>
+        <v>0.60606060606060608</v>
       </c>
       <c r="E4">
         <f>bosqueu!C2</f>
-        <v>0.56688311688311688</v>
+        <v>0.56534336167429688</v>
       </c>
       <c r="F4">
         <f>bosqueu!D2</f>
-        <v>0.61212121212121207</v>
+        <v>0.60606060606060608</v>
       </c>
       <c r="G4" s="1">
         <f>bosqueu!E2</f>
-        <v>0.54564233474908852</v>
+        <v>0.54243651880987798</v>
       </c>
       <c r="H4" s="1">
         <f>bosqueu!F2</f>
-        <v>0.77109274563820018</v>
+        <v>0.77104377104377098</v>
       </c>
       <c r="I4" s="1">
         <f>bosqueu!G2</f>
@@ -1274,7 +1271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>13</v>
       </c>
@@ -1384,14 +1381,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
@@ -1408,21 +1405,21 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2">
-        <v>0.6798361056886949</v>
+        <v>0.68458545972045226</v>
       </c>
       <c r="C2">
-        <v>0.76048642178320625</v>
+        <v>0.76178548419983749</v>
       </c>
       <c r="D2">
-        <v>0.87205872610920321</v>
+        <v>0.87280323338071886</v>
       </c>
       <c r="E2">
-        <v>0.30010773556616671</v>
+        <v>0.2989121800501523</v>
       </c>
     </row>
   </sheetData>
@@ -1431,16 +1428,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>41</v>
       </c>
@@ -1457,21 +1452,21 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>122</v>
       </c>
       <c r="B2">
-        <v>0.45832907888266639</v>
+        <v>0.45730041694952078</v>
       </c>
       <c r="C2">
-        <v>0.41024114498902697</v>
+        <v>0.41003396453199498</v>
       </c>
       <c r="D2">
-        <v>0.64050069866396475</v>
+        <v>0.64033894503770039</v>
       </c>
       <c r="E2">
-        <v>0.62244611382141157</v>
+        <v>0.62263678652123244</v>
       </c>
     </row>
   </sheetData>
@@ -1480,14 +1475,14 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>64</v>
       </c>
@@ -1504,7 +1499,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>15</v>
       </c>
@@ -1527,14 +1522,14 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
@@ -1551,21 +1546,21 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.56643131719760875</v>
+        <v>0.57747296207426224</v>
       </c>
       <c r="C2">
-        <v>0.59821231730879365</v>
+        <v>0.64663383462689228</v>
       </c>
       <c r="D2">
-        <v>0.77344186420751349</v>
+        <v>0.8041354578843618</v>
       </c>
       <c r="E2">
-        <v>0.41244289181922278</v>
+        <v>0.36488384653386541</v>
       </c>
     </row>
   </sheetData>
@@ -1574,14 +1569,14 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>41</v>
       </c>
@@ -1598,21 +1593,21 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>115</v>
       </c>
       <c r="B2">
-        <v>0.4295092022072674</v>
+        <v>0.42935267814997469</v>
       </c>
       <c r="C2">
-        <v>0.35043803160514547</v>
+        <v>0.35045962289335952</v>
       </c>
       <c r="D2">
-        <v>0.59197806682777154</v>
+        <v>0.59199630310784834</v>
       </c>
       <c r="E2">
-        <v>0.65580388352285035</v>
+        <v>0.65578267681329627</v>
       </c>
     </row>
   </sheetData>
@@ -1621,14 +1616,14 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>64</v>
       </c>
@@ -1645,7 +1640,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3</v>
       </c>
@@ -1668,14 +1663,14 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
@@ -1692,21 +1687,21 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>6</v>
       </c>
       <c r="B2">
-        <v>0.77089946186766289</v>
+        <v>0.77556922135398898</v>
       </c>
       <c r="C2">
-        <v>1.8751200753384381</v>
+        <v>1.827375618630338</v>
       </c>
       <c r="D2">
-        <v>1.3693502383752809</v>
+        <v>1.3518045785653849</v>
       </c>
       <c r="E2">
-        <v>-1.171224911562941</v>
+        <v>-1.1159410099306919</v>
       </c>
     </row>
   </sheetData>
@@ -1715,14 +1710,14 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>41</v>
       </c>
@@ -1739,21 +1734,21 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>110</v>
       </c>
       <c r="B2">
-        <v>0.62798222597566722</v>
+        <v>0.6276056324687056</v>
       </c>
       <c r="C2">
-        <v>0.57392416817868541</v>
+        <v>0.57358128035905465</v>
       </c>
       <c r="D2">
-        <v>0.75757782978297705</v>
+        <v>0.75735149062971718</v>
       </c>
       <c r="E2">
-        <v>0.33544605079613887</v>
+        <v>0.33584308487712661</v>
       </c>
     </row>
   </sheetData>
@@ -1762,14 +1757,14 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>64</v>
       </c>
@@ -1786,7 +1781,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>5</v>
       </c>
@@ -1819,23 +1814,23 @@
       <selection sqref="A1:K25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="18.5" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
     <col min="6" max="6" width="34" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" customWidth="1"/>
-    <col min="8" max="8" width="12.83203125" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>14</v>
       </c>
@@ -1867,7 +1862,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>11</v>
       </c>
@@ -1908,33 +1903,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>12</v>
       </c>
       <c r="C4">
         <f>bosqueu!A2</f>
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D4">
         <f>bosqueu!B2</f>
-        <v>0.61212121212121207</v>
+        <v>0.60606060606060608</v>
       </c>
       <c r="E4">
         <f>bosqueu!C2</f>
-        <v>0.56688311688311688</v>
+        <v>0.56534336167429688</v>
       </c>
       <c r="F4">
         <f>bosqueu!D2</f>
-        <v>0.61212121212121207</v>
+        <v>0.60606060606060608</v>
       </c>
       <c r="G4" s="1">
         <f>bosqueu!E2</f>
-        <v>0.54564233474908852</v>
+        <v>0.54243651880987798</v>
       </c>
       <c r="H4" s="1">
         <f>bosqueu!F2</f>
-        <v>0.77109274563820018</v>
+        <v>0.77104377104377098</v>
       </c>
       <c r="I4" s="1">
         <f>bosqueu!G2</f>
@@ -1949,7 +1944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>13</v>
       </c>
@@ -1990,7 +1985,7 @@
         <v>0.81660899653979235</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>15</v>
       </c>
@@ -2013,7 +2008,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>21</v>
       </c>
@@ -2023,15 +2018,15 @@
       </c>
       <c r="D8">
         <f>arbolts!B2</f>
-        <v>0.88857003700225046</v>
+        <v>0.87082129423169974</v>
       </c>
       <c r="E8" s="1">
         <f>arbolts!E2</f>
-        <v>-0.69305130212917132</v>
+        <v>-0.67171571964877375</v>
       </c>
       <c r="F8" s="1">
         <f>arbolts!C2</f>
-        <v>1.4032458894705599</v>
+        <v>1.3855623920021569</v>
       </c>
       <c r="G8" s="1">
         <f>arbolts!F2</f>
@@ -2039,28 +2034,28 @@
       </c>
       <c r="H8" s="1">
         <f>arbolts!D2</f>
-        <v>1.1845868011549681</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1.177099142809201</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>22</v>
       </c>
       <c r="C9">
         <f>bosquets!A2</f>
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D9">
         <f>bosquets!B2</f>
-        <v>0.63279993377906929</v>
+        <v>0.80011335135049144</v>
       </c>
       <c r="E9" s="1">
         <f>bosquets!E2</f>
-        <v>0.22037552312985109</v>
+        <v>0.64018137500931493</v>
       </c>
       <c r="F9" s="1">
         <f>bosquets!C2</f>
-        <v>0.64617347455618035</v>
+        <v>0.62903132060923439</v>
       </c>
       <c r="G9" s="1">
         <f>bosquets!F2</f>
@@ -2068,10 +2063,10 @@
       </c>
       <c r="H9" s="1">
         <f>bosquets!D2</f>
-        <v>0.80384916156961961</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0.22760514127192591</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>23</v>
       </c>
@@ -2081,15 +2076,15 @@
       </c>
       <c r="D10">
         <f>knnts!B2</f>
-        <v>0.64651818574721454</v>
+        <v>0.64651818574721431</v>
       </c>
       <c r="E10" s="1">
         <f>knnts!E2</f>
-        <v>0.14621323287680579</v>
+        <v>0.1462132328768061</v>
       </c>
       <c r="F10" s="1">
         <f>knnts!C2</f>
-        <v>0.70764115059200594</v>
+        <v>0.70764115059200561</v>
       </c>
       <c r="G10" s="1">
         <f>knnts!F2</f>
@@ -2097,10 +2092,10 @@
       </c>
       <c r="H10" s="1">
         <f>knnts!D2</f>
-        <v>0.84121409319625995</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0.84121409319625973</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>24</v>
       </c>
@@ -2123,25 +2118,25 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>25</v>
       </c>
       <c r="C13">
         <f>arboltd!A2</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D13">
         <f>arboltd!B2</f>
-        <v>0.6798361056886949</v>
+        <v>0.68458545972045226</v>
       </c>
       <c r="E13" s="1">
         <f>arboltd!E2</f>
-        <v>0.30010773556616671</v>
+        <v>0.2989121800501523</v>
       </c>
       <c r="F13" s="1">
         <f>arboltd!C2</f>
-        <v>0.76048642178320625</v>
+        <v>0.76178548419983749</v>
       </c>
       <c r="G13" s="1">
         <f>arboltd!F2</f>
@@ -2149,10 +2144,10 @@
       </c>
       <c r="H13" s="1">
         <f>arboltd!D2</f>
-        <v>0.87205872610920321</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0.87280323338071886</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>26</v>
       </c>
@@ -2162,15 +2157,15 @@
       </c>
       <c r="D14">
         <f>bosquetd!B2</f>
-        <v>0.45832907888266639</v>
+        <v>0.45730041694952078</v>
       </c>
       <c r="E14" s="1">
         <f>bosquetd!E2</f>
-        <v>0.62244611382141157</v>
+        <v>0.62263678652123244</v>
       </c>
       <c r="F14" s="1">
         <f>bosquetd!C2</f>
-        <v>0.41024114498902697</v>
+        <v>0.41003396453199498</v>
       </c>
       <c r="G14" s="1">
         <f>bosquetd!F2</f>
@@ -2178,10 +2173,10 @@
       </c>
       <c r="H14" s="1">
         <f>bosquetd!D2</f>
-        <v>0.64050069866396475</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0.64033894503770039</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>27</v>
       </c>
@@ -2210,7 +2205,7 @@
         <v>0.82572113269060754</v>
       </c>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>28</v>
       </c>
@@ -2233,7 +2228,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>29</v>
       </c>
@@ -2243,15 +2238,15 @@
       </c>
       <c r="D18">
         <f>arbolcc!B2</f>
-        <v>0.56643131719760875</v>
+        <v>0.57747296207426224</v>
       </c>
       <c r="E18" s="1">
         <f>arbolcc!E2</f>
-        <v>0.41244289181922278</v>
+        <v>0.36488384653386541</v>
       </c>
       <c r="F18" s="1">
         <f>arbolcc!C2</f>
-        <v>0.59821231730879365</v>
+        <v>0.64663383462689228</v>
       </c>
       <c r="G18" s="1">
         <f>arbolcc!F2</f>
@@ -2259,10 +2254,10 @@
       </c>
       <c r="H18" s="1">
         <f>arbolcc!D2</f>
-        <v>0.77344186420751349</v>
-      </c>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.2">
+        <v>0.8041354578843618</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>30</v>
       </c>
@@ -2272,15 +2267,15 @@
       </c>
       <c r="D19">
         <f>bosquecc!B2</f>
-        <v>0.4295092022072674</v>
+        <v>0.42935267814997469</v>
       </c>
       <c r="E19" s="1">
         <f>bosquecc!E2</f>
-        <v>0.65580388352285035</v>
+        <v>0.65578267681329627</v>
       </c>
       <c r="F19" s="1">
         <f>bosquecc!C2</f>
-        <v>0.35043803160514547</v>
+        <v>0.35045962289335952</v>
       </c>
       <c r="G19" s="1">
         <f>bosquecc!F2</f>
@@ -2288,10 +2283,10 @@
       </c>
       <c r="H19" s="1">
         <f>bosquecc!D2</f>
-        <v>0.59197806682777154</v>
-      </c>
-    </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.2">
+        <v>0.59199630310784834</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>31</v>
       </c>
@@ -2320,7 +2315,7 @@
         <v>0.69288975777381279</v>
       </c>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>32</v>
       </c>
@@ -2343,7 +2338,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>33</v>
       </c>
@@ -2353,15 +2348,15 @@
       </c>
       <c r="D23">
         <f>arbolpp!B2</f>
-        <v>0.77089946186766289</v>
+        <v>0.77556922135398898</v>
       </c>
       <c r="E23" s="1">
         <f>arbolpp!E2</f>
-        <v>-1.171224911562941</v>
+        <v>-1.1159410099306919</v>
       </c>
       <c r="F23" s="1">
         <f>arbolpp!C2</f>
-        <v>1.8751200753384381</v>
+        <v>1.827375618630338</v>
       </c>
       <c r="G23" s="1">
         <f>arbolpp!F2</f>
@@ -2369,7 +2364,7 @@
       </c>
       <c r="H23" s="1">
         <f>arbolpp!D2</f>
-        <v>1.3693502383752809</v>
+        <v>1.3518045785653849</v>
       </c>
       <c r="L23">
         <v>16</v>
@@ -2384,7 +2379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>34</v>
       </c>
@@ -2394,15 +2389,15 @@
       </c>
       <c r="D24">
         <f>bosquepp!B2</f>
-        <v>0.62798222597566722</v>
+        <v>0.6276056324687056</v>
       </c>
       <c r="E24" s="1">
         <f>bosquepp!E2</f>
-        <v>0.33544605079613887</v>
+        <v>0.33584308487712661</v>
       </c>
       <c r="F24" s="1">
         <f>bosquepp!C2</f>
-        <v>0.57392416817868541</v>
+        <v>0.57358128035905465</v>
       </c>
       <c r="G24" s="1">
         <f>bosquepp!F2</f>
@@ -2410,7 +2405,7 @@
       </c>
       <c r="H24" s="1">
         <f>bosquepp!D2</f>
-        <v>0.75757782978297705</v>
+        <v>0.75735149062971718</v>
       </c>
       <c r="L24">
         <f>L23*M24</f>
@@ -2427,7 +2422,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>35</v>
       </c>
@@ -2470,7 +2465,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
       <c r="L26">
         <v>2</v>
       </c>
@@ -2486,7 +2481,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
       <c r="L27">
         <v>3</v>
       </c>
@@ -2502,7 +2497,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
       <c r="L28">
         <v>4</v>
       </c>
@@ -2518,7 +2513,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
       <c r="L29">
         <v>5</v>
       </c>
@@ -2534,7 +2529,7 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
       <c r="L30">
         <v>6</v>
       </c>
@@ -2550,7 +2545,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
       <c r="L31">
         <v>7</v>
       </c>
@@ -2566,7 +2561,7 @@
         <v>0.58333333333333337</v>
       </c>
     </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
       <c r="L32">
         <v>8</v>
       </c>
@@ -2582,7 +2577,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="33" spans="12:16" x14ac:dyDescent="0.2">
+    <row r="33" spans="12:16" x14ac:dyDescent="0.25">
       <c r="L33">
         <v>9</v>
       </c>
@@ -2598,7 +2593,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="34" spans="12:16" x14ac:dyDescent="0.2">
+    <row r="34" spans="12:16" x14ac:dyDescent="0.25">
       <c r="L34">
         <v>10</v>
       </c>
@@ -2614,7 +2609,7 @@
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="35" spans="12:16" x14ac:dyDescent="0.2">
+    <row r="35" spans="12:16" x14ac:dyDescent="0.25">
       <c r="L35">
         <v>11</v>
       </c>
@@ -2630,7 +2625,7 @@
         <v>0.91666666666666663</v>
       </c>
     </row>
-    <row r="36" spans="12:16" x14ac:dyDescent="0.2">
+    <row r="36" spans="12:16" x14ac:dyDescent="0.25">
       <c r="L36">
         <v>12</v>
       </c>
@@ -2912,37 +2907,41 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DE89837-C912-794F-A747-38AF6996C5DA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" customWidth="1"/>
-    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>14</v>
       </c>
@@ -2950,31 +2949,22 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="H2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>11</v>
       </c>
@@ -2982,81 +2972,57 @@
         <f>arbolu!A2</f>
         <v>3</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <f>arbolu!B2</f>
         <v>0.61212121212121207</v>
       </c>
-      <c r="E3">
-        <f>arbolu!C2</f>
-        <v>0.41197063805759448</v>
-      </c>
-      <c r="F3">
-        <f>arbolu!D2</f>
-        <v>0.61212121212121207</v>
-      </c>
-      <c r="G3" s="1">
-        <f>arbolu!E2</f>
-        <v>0.48260789715335167</v>
-      </c>
-      <c r="H3" s="1">
+      <c r="E3" s="1">
         <f>arbolu!F2</f>
         <v>0.77411692684419953</v>
       </c>
-      <c r="I3" s="1">
+      <c r="F3" s="1">
         <f>arbolu!G2</f>
         <v>0</v>
       </c>
-      <c r="J3" s="1">
+      <c r="G3" s="1">
         <f>arbolu!H2</f>
         <v>0</v>
       </c>
-      <c r="K3" s="1">
+      <c r="H3" s="1">
         <f>arbolu!I2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>12</v>
       </c>
       <c r="C4">
         <f>bosqueu!A2</f>
-        <v>108</v>
-      </c>
-      <c r="D4">
+        <v>110</v>
+      </c>
+      <c r="D4" s="1">
         <f>bosqueu!B2</f>
-        <v>0.61212121212121207</v>
-      </c>
-      <c r="E4">
-        <f>bosqueu!C2</f>
-        <v>0.56688311688311688</v>
-      </c>
-      <c r="F4">
-        <f>bosqueu!D2</f>
-        <v>0.61212121212121207</v>
-      </c>
-      <c r="G4" s="1">
-        <f>bosqueu!E2</f>
-        <v>0.54564233474908852</v>
-      </c>
-      <c r="H4" s="1">
+        <v>0.60606060606060608</v>
+      </c>
+      <c r="E4" s="1">
         <f>bosqueu!F2</f>
-        <v>0.77109274563820018</v>
-      </c>
-      <c r="I4" s="1">
+        <v>0.77104377104377098</v>
+      </c>
+      <c r="F4" s="1">
         <f>bosqueu!G2</f>
         <v>0</v>
       </c>
-      <c r="J4" s="1">
+      <c r="G4" s="1">
         <f>bosqueu!H2</f>
         <v>0</v>
       </c>
-      <c r="K4" s="1">
+      <c r="H4" s="1">
         <f>bosqueu!I2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>13</v>
       </c>
@@ -3064,40 +3030,28 @@
         <f>knnu!A2</f>
         <v>23</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <f>knnu!B2</f>
         <v>38</v>
       </c>
-      <c r="E5">
-        <f>knnu!C2</f>
-        <v>0.55882352941176472</v>
-      </c>
-      <c r="F5">
-        <f>knnu!D2</f>
-        <v>0</v>
-      </c>
-      <c r="G5" s="1">
-        <f>knnu!E2</f>
-        <v>0.55882352941176472</v>
-      </c>
-      <c r="H5" s="1">
+      <c r="E5" s="1">
         <f>knnu!F2</f>
         <v>0.31228373702422152</v>
       </c>
-      <c r="I5" s="1">
+      <c r="F5" s="1">
         <f>knnu!G2</f>
         <v>0.55882352941176472</v>
       </c>
-      <c r="J5" s="1">
+      <c r="G5" s="1">
         <f>knnu!H2</f>
         <v>0.40066592674805768</v>
       </c>
-      <c r="K5" s="1">
+      <c r="H5" s="1">
         <f>knnu!I2</f>
         <v>0.81660899653979235</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>15</v>
       </c>
@@ -3120,7 +3074,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>21</v>
       </c>
@@ -3130,55 +3084,55 @@
       </c>
       <c r="D8">
         <f>arbolts!B2</f>
-        <v>0.88857003700225046</v>
+        <v>0.87082129423169974</v>
       </c>
       <c r="E8" s="1">
         <f>arbolts!E2</f>
-        <v>-0.69305130212917132</v>
+        <v>-0.67171571964877375</v>
       </c>
       <c r="F8" s="1">
         <f>arbolts!C2</f>
-        <v>1.4032458894705599</v>
+        <v>1.3855623920021569</v>
       </c>
       <c r="G8" s="1">
-        <f>arbolts!F2</f>
-        <v>0</v>
+        <f>arbolts!E2</f>
+        <v>-0.67171571964877375</v>
       </c>
       <c r="H8" s="1">
         <f>arbolts!D2</f>
-        <v>1.1845868011549681</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1.177099142809201</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>22</v>
       </c>
       <c r="C9">
         <f>bosquets!A2</f>
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D9">
         <f>bosquets!B2</f>
-        <v>0.63279993377906929</v>
+        <v>0.80011335135049144</v>
       </c>
       <c r="E9" s="1">
         <f>bosquets!E2</f>
-        <v>0.22037552312985109</v>
+        <v>0.64018137500931493</v>
       </c>
       <c r="F9" s="1">
         <f>bosquets!C2</f>
-        <v>0.64617347455618035</v>
+        <v>0.62903132060923439</v>
       </c>
       <c r="G9" s="1">
-        <f>bosquets!F2</f>
-        <v>0</v>
+        <f>bosquets!E2</f>
+        <v>0.64018137500931493</v>
       </c>
       <c r="H9" s="1">
         <f>bosquets!D2</f>
-        <v>0.80384916156961961</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0.22760514127192591</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>23</v>
       </c>
@@ -3188,26 +3142,26 @@
       </c>
       <c r="D10">
         <f>knnts!B2</f>
-        <v>0.64651818574721454</v>
+        <v>0.64651818574721431</v>
       </c>
       <c r="E10" s="1">
         <f>knnts!E2</f>
-        <v>0.14621323287680579</v>
+        <v>0.1462132328768061</v>
       </c>
       <c r="F10" s="1">
         <f>knnts!C2</f>
-        <v>0.70764115059200594</v>
+        <v>0.70764115059200561</v>
       </c>
       <c r="G10" s="1">
-        <f>knnts!F2</f>
-        <v>0</v>
+        <f>knnts!E2</f>
+        <v>0.1462132328768061</v>
       </c>
       <c r="H10" s="1">
         <f>knnts!D2</f>
-        <v>0.84121409319625995</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0.84121409319625973</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>24</v>
       </c>
@@ -3230,36 +3184,36 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>25</v>
       </c>
       <c r="C13">
         <f>arboltd!A2</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D13">
         <f>arboltd!B2</f>
-        <v>0.6798361056886949</v>
+        <v>0.68458545972045226</v>
       </c>
       <c r="E13" s="1">
         <f>arboltd!E2</f>
-        <v>0.30010773556616671</v>
+        <v>0.2989121800501523</v>
       </c>
       <c r="F13" s="1">
         <f>arboltd!C2</f>
-        <v>0.76048642178320625</v>
+        <v>0.76178548419983749</v>
       </c>
       <c r="G13" s="1">
-        <f>arboltd!F2</f>
-        <v>0</v>
+        <f>arboltd!E2</f>
+        <v>0.2989121800501523</v>
       </c>
       <c r="H13" s="1">
         <f>arboltd!D2</f>
-        <v>0.87205872610920321</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0.87280323338071886</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>26</v>
       </c>
@@ -3269,26 +3223,26 @@
       </c>
       <c r="D14">
         <f>bosquetd!B2</f>
-        <v>0.45832907888266639</v>
+        <v>0.45730041694952078</v>
       </c>
       <c r="E14" s="1">
         <f>bosquetd!E2</f>
-        <v>0.62244611382141157</v>
+        <v>0.62263678652123244</v>
       </c>
       <c r="F14" s="1">
         <f>bosquetd!C2</f>
-        <v>0.41024114498902697</v>
+        <v>0.41003396453199498</v>
       </c>
       <c r="G14" s="1">
-        <f>bosquetd!F2</f>
-        <v>0</v>
+        <f>bosquetd!E2</f>
+        <v>0.62263678652123244</v>
       </c>
       <c r="H14" s="1">
         <f>bosquetd!D2</f>
-        <v>0.64050069866396475</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0.64033894503770039</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>27</v>
       </c>
@@ -3309,15 +3263,15 @@
         <v>0.68181538897185989</v>
       </c>
       <c r="G15" s="1">
-        <f>knntd!F2</f>
-        <v>0</v>
+        <f>knntd!E2</f>
+        <v>0.37251040538711189</v>
       </c>
       <c r="H15" s="1">
         <f>knntd!D2</f>
         <v>0.82572113269060754</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>28</v>
       </c>
@@ -3340,7 +3294,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>29</v>
       </c>
@@ -3350,26 +3304,26 @@
       </c>
       <c r="D18">
         <f>arbolcc!B2</f>
-        <v>0.56643131719760875</v>
+        <v>0.57747296207426224</v>
       </c>
       <c r="E18" s="1">
         <f>arbolcc!E2</f>
-        <v>0.41244289181922278</v>
+        <v>0.36488384653386541</v>
       </c>
       <c r="F18" s="1">
         <f>arbolcc!C2</f>
-        <v>0.59821231730879365</v>
+        <v>0.64663383462689228</v>
       </c>
       <c r="G18" s="1">
-        <f>arbolcc!F2</f>
-        <v>0</v>
+        <f>arbolcc!E2</f>
+        <v>0.36488384653386541</v>
       </c>
       <c r="H18" s="1">
         <f>arbolcc!D2</f>
-        <v>0.77344186420751349</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+        <v>0.8041354578843618</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>30</v>
       </c>
@@ -3379,26 +3333,26 @@
       </c>
       <c r="D19">
         <f>bosquecc!B2</f>
-        <v>0.4295092022072674</v>
+        <v>0.42935267814997469</v>
       </c>
       <c r="E19" s="1">
         <f>bosquecc!E2</f>
-        <v>0.65580388352285035</v>
+        <v>0.65578267681329627</v>
       </c>
       <c r="F19" s="1">
         <f>bosquecc!C2</f>
-        <v>0.35043803160514547</v>
+        <v>0.35045962289335952</v>
       </c>
       <c r="G19" s="1">
-        <f>bosquecc!F2</f>
-        <v>0</v>
+        <f>bosquecc!E2</f>
+        <v>0.65578267681329627</v>
       </c>
       <c r="H19" s="1">
         <f>bosquecc!D2</f>
-        <v>0.59197806682777154</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+        <v>0.59199630310784834</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>31</v>
       </c>
@@ -3419,15 +3373,15 @@
         <v>0.48009621642785288</v>
       </c>
       <c r="G20" s="1">
-        <f>knncc!F2</f>
-        <v>0</v>
+        <f>knncc!E2</f>
+        <v>0.5284551380655178</v>
       </c>
       <c r="H20" s="1">
         <f>knncc!D2</f>
         <v>0.69288975777381279</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>32</v>
       </c>
@@ -3450,7 +3404,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>33</v>
       </c>
@@ -3460,26 +3414,26 @@
       </c>
       <c r="D23">
         <f>arbolpp!B2</f>
-        <v>0.77089946186766289</v>
+        <v>0.77556922135398898</v>
       </c>
       <c r="E23" s="1">
         <f>arbolpp!E2</f>
-        <v>-1.171224911562941</v>
+        <v>-1.1159410099306919</v>
       </c>
       <c r="F23" s="1">
         <f>arbolpp!C2</f>
-        <v>1.8751200753384381</v>
+        <v>1.827375618630338</v>
       </c>
       <c r="G23" s="1">
-        <f>arbolpp!F2</f>
-        <v>0</v>
+        <f>arbolpp!E2</f>
+        <v>-1.1159410099306919</v>
       </c>
       <c r="H23" s="1">
         <f>arbolpp!D2</f>
-        <v>1.3693502383752809</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+        <v>1.3518045785653849</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>34</v>
       </c>
@@ -3489,26 +3443,26 @@
       </c>
       <c r="D24">
         <f>bosquepp!B2</f>
-        <v>0.62798222597566722</v>
+        <v>0.6276056324687056</v>
       </c>
       <c r="E24" s="1">
         <f>bosquepp!E2</f>
-        <v>0.33544605079613887</v>
+        <v>0.33584308487712661</v>
       </c>
       <c r="F24" s="1">
         <f>bosquepp!C2</f>
-        <v>0.57392416817868541</v>
+        <v>0.57358128035905465</v>
       </c>
       <c r="G24" s="1">
-        <f>bosquepp!F2</f>
-        <v>0</v>
+        <f>bosquepp!E2</f>
+        <v>0.33584308487712661</v>
       </c>
       <c r="H24" s="1">
         <f>bosquepp!D2</f>
-        <v>0.75757782978297705</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+        <v>0.75735149062971718</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>35</v>
       </c>
@@ -3529,8 +3483,8 @@
         <v>0.83152824107238332</v>
       </c>
       <c r="G25" s="1">
-        <f>knnpp!F2</f>
-        <v>0</v>
+        <f>knnpp!E2</f>
+        <v>3.716308335154872E-2</v>
       </c>
       <c r="H25" s="1">
         <f>knnpp!D2</f>
@@ -3634,7 +3588,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G5">
+  <conditionalFormatting sqref="D3:D5">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -3694,7 +3648,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:H5">
+  <conditionalFormatting sqref="E3:E5">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -3754,7 +3708,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I5">
+  <conditionalFormatting sqref="F3:F5">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -3766,7 +3720,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J5">
+  <conditionalFormatting sqref="G3:G5">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -3778,7 +3732,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K5">
+  <conditionalFormatting sqref="H3:H5">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -3802,69 +3756,6 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.83203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>3</v>
-      </c>
-      <c r="B2">
-        <v>0.61212121212121207</v>
-      </c>
-      <c r="C2">
-        <v>0.41197063805759448</v>
-      </c>
-      <c r="D2">
-        <v>0.61212121212121207</v>
-      </c>
-      <c r="E2">
-        <v>0.48260789715335167</v>
-      </c>
-      <c r="F2">
-        <v>0.77411692684419953</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -3872,9 +3763,69 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>0.61212121212121207</v>
+      </c>
+      <c r="C2">
+        <v>0.41197063805759448</v>
+      </c>
+      <c r="D2">
+        <v>0.61212121212121207</v>
+      </c>
+      <c r="E2">
+        <v>0.48260789715335167</v>
+      </c>
+      <c r="F2">
+        <v>0.77411692684419953</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>41</v>
       </c>
@@ -3894,24 +3845,24 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B2">
-        <v>0.61212121212121207</v>
+        <v>0.60606060606060608</v>
       </c>
       <c r="C2">
-        <v>0.56688311688311688</v>
+        <v>0.56534336167429688</v>
       </c>
       <c r="D2">
-        <v>0.61212121212121207</v>
+        <v>0.60606060606060608</v>
       </c>
       <c r="E2">
-        <v>0.54564233474908852</v>
+        <v>0.54243651880987798</v>
       </c>
       <c r="F2">
-        <v>0.77109274563820018</v>
+        <v>0.77104377104377098</v>
       </c>
     </row>
   </sheetData>
@@ -3920,14 +3871,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>47</v>
       </c>
@@ -3956,7 +3909,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>23</v>
       </c>
@@ -3991,16 +3944,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
@@ -4017,21 +3970,21 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.88857003700225046</v>
+        <v>0.87082129423169974</v>
       </c>
       <c r="C2">
-        <v>1.4032458894705599</v>
+        <v>1.3855623920021569</v>
       </c>
       <c r="D2">
-        <v>1.1845868011549681</v>
+        <v>1.177099142809201</v>
       </c>
       <c r="E2">
-        <v>-0.69305130212917132</v>
+        <v>-0.67171571964877375</v>
       </c>
     </row>
   </sheetData>
@@ -4040,22 +3993,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView zoomScale="270" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>41</v>
       </c>
@@ -4072,21 +4017,21 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B2">
-        <v>0.63279993377906929</v>
+        <v>0.80011335135049144</v>
       </c>
       <c r="C2">
-        <v>0.64617347455618035</v>
+        <v>0.62903132060923439</v>
       </c>
       <c r="D2">
-        <v>0.80384916156961961</v>
+        <v>0.22760514127192591</v>
       </c>
       <c r="E2">
-        <v>0.22037552312985109</v>
+        <v>0.64018137500931493</v>
       </c>
     </row>
   </sheetData>
@@ -4095,14 +4040,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>64</v>
       </c>
@@ -4119,21 +4064,21 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>23</v>
       </c>
       <c r="B2">
-        <v>0.64651818574721454</v>
+        <v>0.64651818574721431</v>
       </c>
       <c r="C2">
-        <v>0.70764115059200594</v>
+        <v>0.70764115059200561</v>
       </c>
       <c r="D2">
-        <v>0.84121409319625995</v>
+        <v>0.84121409319625973</v>
       </c>
       <c r="E2">
-        <v>0.14621323287680579</v>
+        <v>0.1462132328768061</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
terminando el word del articulo
</commit_message>
<xml_diff>
--- a/resultadospython.xlsx
+++ b/resultadospython.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a57f4c5e645b2417/1 A NMI/3 InvestigacionMia/F Métodos predictivos con ML/A Codigo/Comparacion_de_metodos_predictivos/crispy-invention_metodos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="155" documentId="11_2A9B9621388861AE7BA9BACABEB497E22FE56990" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A14542F-885F-4E7A-9782-0B77A56A1AB3}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="11_76C9C414D995F498669106D91195431FBB6D9F04" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4103A56-AD9E-40A4-BCBF-0CA3DBFE8F94}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="894" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,24 +58,99 @@
     <t>Algoritmo</t>
   </si>
   <si>
+    <t>Exactitud</t>
+  </si>
+  <si>
+    <t>Precisión</t>
+  </si>
+  <si>
+    <t>Sensibilidad</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>ROC/AUC</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>RMSE</t>
+  </si>
+  <si>
+    <t>MAE</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>MSE</t>
+  </si>
+  <si>
+    <t>Árbol de desición</t>
+  </si>
+  <si>
+    <t>Tensión sistólica</t>
+  </si>
+  <si>
+    <t>Bosque aleatorio</t>
+  </si>
+  <si>
+    <t>KNN</t>
+  </si>
+  <si>
+    <t>Tensión diastólica</t>
+  </si>
+  <si>
     <t>Modelo</t>
   </si>
   <si>
+    <t>arbolts</t>
+  </si>
+  <si>
+    <t>bosquets</t>
+  </si>
+  <si>
+    <t>Circunferencia de cintura</t>
+  </si>
+  <si>
+    <t>knnts</t>
+  </si>
+  <si>
+    <t>Perímetro de pantorrilla</t>
+  </si>
+  <si>
+    <t>arboltd</t>
+  </si>
+  <si>
+    <t>bosquetd</t>
+  </si>
+  <si>
+    <t>knntd</t>
+  </si>
+  <si>
+    <t>arbolcc</t>
+  </si>
+  <si>
+    <t>bosquecc</t>
+  </si>
+  <si>
+    <t>knncc</t>
+  </si>
+  <si>
+    <t>arbolpp</t>
+  </si>
+  <si>
+    <t>bosquepp</t>
+  </si>
+  <si>
+    <t>knnpp</t>
+  </si>
+  <si>
     <t>Hiperparámetro</t>
   </si>
   <si>
-    <t>RMSE</t>
-  </si>
-  <si>
-    <t>MAE</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>MSE</t>
-  </si>
-  <si>
     <t>arbol</t>
   </si>
   <si>
@@ -97,57 +172,6 @@
     <t>pp</t>
   </si>
   <si>
-    <t>arbolts</t>
-  </si>
-  <si>
-    <t>bosquets</t>
-  </si>
-  <si>
-    <t>knnts</t>
-  </si>
-  <si>
-    <t>Exactitud</t>
-  </si>
-  <si>
-    <t>Precisión</t>
-  </si>
-  <si>
-    <t>Sensibilidad</t>
-  </si>
-  <si>
-    <t>F1</t>
-  </si>
-  <si>
-    <t>ROC/AUC</t>
-  </si>
-  <si>
-    <t>arboltd</t>
-  </si>
-  <si>
-    <t>bosquetd</t>
-  </si>
-  <si>
-    <t>knntd</t>
-  </si>
-  <si>
-    <t>arbolcc</t>
-  </si>
-  <si>
-    <t>bosquecc</t>
-  </si>
-  <si>
-    <t>knncc</t>
-  </si>
-  <si>
-    <t>arbolpp</t>
-  </si>
-  <si>
-    <t>bosquepp</t>
-  </si>
-  <si>
-    <t>knnpp</t>
-  </si>
-  <si>
     <t>Profundidad óptima</t>
   </si>
   <si>
@@ -344,30 +368,6 @@
   </si>
   <si>
     <t>MSE knnpp</t>
-  </si>
-  <si>
-    <t>Árbol de desición</t>
-  </si>
-  <si>
-    <t>Bosque aleatorio</t>
-  </si>
-  <si>
-    <t>KNN</t>
-  </si>
-  <si>
-    <t>Variable</t>
-  </si>
-  <si>
-    <t>Tensión sistólica</t>
-  </si>
-  <si>
-    <t>Tensión diastólica</t>
-  </si>
-  <si>
-    <t>Circunferencia de cintura</t>
-  </si>
-  <si>
-    <t>Perímetro de pantorrilla</t>
   </si>
 </sst>
 </file>
@@ -383,15 +383,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -408,21 +408,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -505,34 +490,62 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="9">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
@@ -588,15 +601,15 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{88D99256-C63A-4D04-9629-F864D1716766}" name="u_2" displayName="u_2" ref="A1:F4" totalsRowShown="0">
-  <autoFilter ref="A1:F4" xr:uid="{88D99256-C63A-4D04-9629-F864D1716766}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="u_2" displayName="u_2" ref="A1:F4" totalsRowShown="0">
+  <autoFilter ref="A1:F4" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{352449D1-F325-49AF-9164-833651ACCAB1}" name="Algoritmo"/>
-    <tableColumn id="3" xr3:uid="{460D246D-C116-4EEC-AF8A-449AB316CE77}" name="Exactitud"/>
-    <tableColumn id="4" xr3:uid="{F0B54C80-E8B7-4BFF-94CB-774A659F6BAF}" name="Precisión"/>
-    <tableColumn id="5" xr3:uid="{7898EA07-5551-493E-98DA-F7FA9BC97458}" name="Sensibilidad"/>
-    <tableColumn id="6" xr3:uid="{206830FD-2825-4922-AD99-8467E9BCFCB4}" name="F1"/>
-    <tableColumn id="7" xr3:uid="{ADCC9360-8F38-4885-9C66-1B03E1711E28}" name="ROC/AUC"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Algoritmo"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Exactitud" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Precisión" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Sensibilidad" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="F1" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="ROC/AUC" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -659,30 +672,30 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{96038980-F2B6-4B8C-A618-0F5D3CB02986}" name="Tabla18" displayName="Tabla18" ref="H1:M13" totalsRowShown="0">
-  <autoFilter ref="H1:M13" xr:uid="{96038980-F2B6-4B8C-A618-0F5D3CB02986}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Tabla18" displayName="Tabla18" ref="H1:M13" totalsRowShown="0">
+  <autoFilter ref="H1:M13" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{6EF7B2FD-A0ED-4E59-903A-707BD537323C}" name="Variable"/>
-    <tableColumn id="2" xr3:uid="{89427F00-1388-4D60-BBFC-163B56330D33}" name="Algoritmo"/>
-    <tableColumn id="3" xr3:uid="{357AF3AC-7521-4D8E-AFAF-3AA20213E257}" name="RMSE" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{856A3D4D-212B-483B-97BC-1A955D6FD203}" name="MAE" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{7E3A141B-912F-4114-A861-0CDBD501DC94}" name="R2" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{15BA2E9C-B099-4D25-A92E-791C7D02FC0F}" name="MSE" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Variable"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Algoritmo"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="RMSE" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="MAE" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="R2" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="MSE" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="u" displayName="u" ref="A1:F4" totalsRowShown="0">
-  <autoFilter ref="A1:F4" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="u" displayName="u" ref="A1:F4" totalsRowShown="0">
+  <autoFilter ref="A1:F4" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Algoritmo"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Exactitud"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Precisión"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Sensibilidad"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="F1"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="ROC/AUC"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Algoritmo"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="Exactitud"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="Precisión"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="Sensibilidad"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="F1"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0800-000007000000}" name="ROC/AUC"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -954,7 +967,7 @@
   <dimension ref="A1:M70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M13" sqref="H1:M13"/>
+      <selection sqref="A1:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -971,231 +984,231 @@
     <col min="12" max="13" width="7.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>100</v>
+        <v>6</v>
       </c>
       <c r="I1" t="s">
         <v>0</v>
       </c>
       <c r="J1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="K1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="L1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="M1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B2">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1">
         <f>arbolu!B2</f>
         <v>0.61212121212121207</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <f>arbolu!C2</f>
         <v>0.41197063805759448</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <f>arbolu!D2</f>
         <v>0.61212121212121207</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <f>arbolu!E2</f>
         <v>0.48260789715335167</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="1">
         <f>arbolu!F2</f>
         <v>0.77411692684419953</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="J2" s="2">
+      <c r="H2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="1">
         <v>1.177099142809201</v>
       </c>
-      <c r="K2" s="5">
+      <c r="K2" s="4">
         <v>0.87082129423169974</v>
       </c>
-      <c r="L2" s="5">
+      <c r="L2" s="4">
         <v>-0.67171571964877375</v>
       </c>
-      <c r="M2" s="6">
+      <c r="M2" s="5">
         <v>1.3855623920021569</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B3">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1">
         <f>bosqueu!B2</f>
         <v>0.60606060606060608</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <f>bosqueu!C2</f>
         <v>0.56534336167429688</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <f>bosqueu!D2</f>
         <v>0.60606060606060608</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <f>bosqueu!E2</f>
         <v>0.54243651880987798</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <f>bosqueu!F2</f>
         <v>0.77104377104377098</v>
       </c>
-      <c r="H3" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="J3" s="2">
+      <c r="H3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="1">
         <v>0.80011335135049144</v>
       </c>
-      <c r="K3" s="9">
+      <c r="K3" s="1">
         <v>0.62903132060923439</v>
       </c>
-      <c r="L3" s="9">
+      <c r="L3" s="1">
         <v>0.22760514127192591</v>
       </c>
-      <c r="M3" s="10">
+      <c r="M3" s="7">
         <v>0.64018137500931493</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B4">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1">
         <f>knnu!B2</f>
         <v>0.62424242424242427</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <f>knnu!C2</f>
         <v>0.38967860422405881</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <f>knnu!D2</f>
         <v>0.62424242424242427</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <f>knnu!E2</f>
         <v>0.47982813206693797</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="1">
         <f>knnu!F2</f>
         <v>0.78112029384756654</v>
       </c>
-      <c r="H4" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="J4" s="2">
+      <c r="H4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="1">
         <v>0.84121409319625973</v>
       </c>
-      <c r="K4" s="13">
+      <c r="K4" s="10">
         <v>0.64651818574721431</v>
       </c>
-      <c r="L4" s="13">
+      <c r="L4" s="10">
         <v>0.1462132328768061</v>
       </c>
-      <c r="M4" s="14">
+      <c r="M4" s="11">
         <v>0.70764115059200561</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H5" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="J5" s="5">
+      <c r="H5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="4">
         <v>0.87280323338071886</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5" s="4">
         <v>0.68458545972045226</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="4">
         <v>0.2989121800501523</v>
       </c>
-      <c r="M5" s="6">
+      <c r="M5" s="5">
         <v>0.76178548419983749</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="J6" s="9">
+        <v>10</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="1">
         <v>0.64033894503770039</v>
       </c>
-      <c r="K6" s="9">
+      <c r="K6" s="1">
         <v>0.45730041694952078</v>
       </c>
-      <c r="L6" s="9">
+      <c r="L6" s="1">
         <v>0.62263678652123244</v>
       </c>
-      <c r="M6" s="10">
+      <c r="M6" s="7">
         <v>0.41003396453199498</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B7">
         <f>arbolts!B2</f>
@@ -1213,28 +1226,28 @@
         <f>arbolts!E2</f>
         <v>1.3855623920021569</v>
       </c>
-      <c r="H7" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="J7" s="13">
+      <c r="H7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="10">
         <v>0.82572113269060754</v>
       </c>
-      <c r="K7" s="13">
+      <c r="K7" s="10">
         <v>0.62201029721223688</v>
       </c>
-      <c r="L7" s="13">
+      <c r="L7" s="10">
         <v>0.37251040538711189</v>
       </c>
-      <c r="M7" s="14">
+      <c r="M7" s="11">
         <v>0.68181538897185989</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B8">
         <f>bosquets!B2</f>
@@ -1252,28 +1265,28 @@
         <f>bosquets!E2</f>
         <v>0.64018137500931493</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="J8" s="5">
+      <c r="H8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="4">
         <v>0.8041354578843618</v>
       </c>
-      <c r="K8" s="5">
+      <c r="K8" s="4">
         <v>0.57747296207426224</v>
       </c>
-      <c r="L8" s="5">
+      <c r="L8" s="4">
         <v>0.36488384653386541</v>
       </c>
-      <c r="M8" s="6">
+      <c r="M8" s="5">
         <v>0.64663383462689228</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B9">
         <f>knnts!B2</f>
@@ -1291,77 +1304,77 @@
         <f>knnts!E2</f>
         <v>0.70764115059200561</v>
       </c>
-      <c r="H9" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="J9" s="9">
+      <c r="H9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J9" s="1">
         <v>0.59199630310784834</v>
       </c>
-      <c r="K9" s="9">
+      <c r="K9" s="1">
         <v>0.42935267814997469</v>
       </c>
-      <c r="L9" s="9">
+      <c r="L9" s="1">
         <v>0.65578267681329627</v>
       </c>
-      <c r="M9" s="10">
+      <c r="M9" s="7">
         <v>0.35045962289335952</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H10" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="I10" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="J10" s="13">
+    <row r="10" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H10" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" s="10">
         <v>0.69288975777381279</v>
       </c>
-      <c r="K10" s="13">
+      <c r="K10" s="10">
         <v>0.53264070017665743</v>
       </c>
-      <c r="L10" s="13">
+      <c r="L10" s="10">
         <v>0.5284551380655178</v>
       </c>
-      <c r="M10" s="14">
+      <c r="M10" s="11">
         <v>0.48009621642785288</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>6</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="J11" s="5">
+        <v>10</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" s="4">
         <v>1.3518045785653849</v>
       </c>
-      <c r="K11" s="5">
+      <c r="K11" s="4">
         <v>0.77556922135398898</v>
       </c>
-      <c r="L11" s="5">
+      <c r="L11" s="4">
         <v>-1.1159410099306919</v>
       </c>
-      <c r="M11" s="6">
+      <c r="M11" s="5">
         <v>1.827375618630338</v>
       </c>
     </row>
@@ -1385,26 +1398,26 @@
         <f>arboltd!E2</f>
         <v>0.76178548419983749</v>
       </c>
-      <c r="H12" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="I12" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="J12" s="9">
+      <c r="H12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" t="s">
+        <v>13</v>
+      </c>
+      <c r="J12" s="1">
         <v>0.75735149062971718</v>
       </c>
-      <c r="K12" s="9">
+      <c r="K12" s="1">
         <v>0.6276056324687056</v>
       </c>
-      <c r="L12" s="9">
+      <c r="L12" s="1">
         <v>0.33584308487712661</v>
       </c>
-      <c r="M12" s="10">
+      <c r="M12" s="7">
         <v>0.57358128035905465</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1424,22 +1437,22 @@
         <f>bosquetd!E2</f>
         <v>0.41003396453199498</v>
       </c>
-      <c r="H13" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="I13" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="J13" s="13">
+      <c r="H13" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" s="10">
         <v>0.91188170344205466</v>
       </c>
-      <c r="K13" s="13">
+      <c r="K13" s="10">
         <v>0.75577833591194044</v>
       </c>
-      <c r="L13" s="13">
+      <c r="L13" s="10">
         <v>3.716308335154872E-2</v>
       </c>
-      <c r="M13" s="14">
+      <c r="M13" s="11">
         <v>0.83152824107238332</v>
       </c>
     </row>
@@ -1466,21 +1479,21 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E16" t="s">
-        <v>6</v>
-      </c>
-      <c r="I16" s="15"/>
+        <v>10</v>
+      </c>
+      <c r="I16" s="12"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -1547,19 +1560,19 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D21" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E21" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1630,30 +1643,30 @@
         <v>0</v>
       </c>
       <c r="B43" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C43" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="D43" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E43" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F43" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G43" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="B44" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="C44">
         <f>arbolts!A2</f>
@@ -1678,10 +1691,10 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="B45" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="C45">
         <f>bosquets!A2</f>
@@ -1706,10 +1719,10 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="B46" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="C46">
         <f>knnts!A2</f>
@@ -1734,10 +1747,10 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="B47" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="C47">
         <f>arboltd!A2</f>
@@ -1762,10 +1775,10 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="B48" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="C48">
         <f>bosquetd!A2</f>
@@ -1790,10 +1803,10 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="B49" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="C49">
         <f>knntd!A2</f>
@@ -1818,10 +1831,10 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="B50" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="C50">
         <f>arbolcc!A2</f>
@@ -1846,10 +1859,10 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="B51" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="C51">
         <f>bosquecc!A2</f>
@@ -1874,10 +1887,10 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="B52" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="C52">
         <f>knncc!A2</f>
@@ -1902,10 +1915,10 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="B53" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="C53">
         <f>arbolpp!A2</f>
@@ -1930,10 +1943,10 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="B54" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="C54">
         <f>bosquepp!A2</f>
@@ -1958,10 +1971,10 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="B55" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="C55">
         <f>knnpp!A2</f>
@@ -1986,21 +1999,21 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B65" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C65" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D65" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="B66">
         <f>arbolts!A2</f>
@@ -2009,7 +2022,7 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B67">
         <f>arbolts!B2</f>
@@ -2018,7 +2031,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B68">
         <f>arbolts!C2</f>
@@ -2027,7 +2040,7 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B69">
         <f>arbolts!A5</f>
@@ -2036,7 +2049,7 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B70">
         <f>arbolts!B5</f>
@@ -2067,20 +2080,20 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>52</v>
+      <c r="A1" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2114,20 +2127,20 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>56</v>
+      <c r="A1" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2161,20 +2174,20 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>60</v>
+      <c r="A1" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2208,20 +2221,20 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>64</v>
+      <c r="A1" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2255,20 +2268,20 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>68</v>
+      <c r="A1" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2302,20 +2315,20 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>72</v>
+      <c r="A1" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2349,20 +2362,20 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>76</v>
+      <c r="A1" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2396,20 +2409,20 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>80</v>
+      <c r="A1" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2443,20 +2456,20 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>84</v>
+      <c r="A1" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2490,20 +2503,20 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>88</v>
+      <c r="A1" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2549,24 +2562,24 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>97</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <f>arbolu!B2</f>
@@ -2591,7 +2604,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>98</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <f>bosqueu!B2</f>
@@ -2616,7 +2629,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <f>knnu!B2</f>
@@ -2656,20 +2669,20 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>92</v>
+      <c r="A1" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2703,20 +2716,20 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>96</v>
+      <c r="A1" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2801,30 +2814,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>36</v>
+      <c r="A1" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2861,23 +2872,23 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>42</v>
+      <c r="A1" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2914,23 +2925,23 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>48</v>
+      <c r="A1" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>